<commit_message>
Adding notes to the third level of the spread vs. usage analysis
</commit_message>
<xml_diff>
--- a/untl-bs/data/SpreadVsUsage-2022-09-15.xlsx
+++ b/untl-bs/data/SpreadVsUsage-2022-09-15.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hjones\Documents\GitHub\portal-leading\untl-bs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2294D152-EBD3-46C2-ADB7-6EDF091744D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C27BBE6-654C-4403-AD4C-CA356B0C7791}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{EC6FB916-47AD-4345-B293-575366B1C3FF}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3979" uniqueCount="2420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3980" uniqueCount="2420">
   <si>
     <t>occurrenceCount</t>
   </si>
@@ -7363,7 +7363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7424,6 +7424,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7742,8 +7745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6320CEFF-DE98-407B-8500-3FF6B38EFF91}">
   <dimension ref="A1:C4823"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A909" workbookViewId="0">
+      <selection activeCell="A929" sqref="A929:B943"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="4" x14ac:dyDescent="0.25"/>
@@ -33326,22 +33329,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFD2735-90EA-4E93-A47B-4BEF3700C1A2}">
   <dimension ref="A1:L664"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F252" sqref="F252"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="G189" sqref="G189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="6" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="10" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="10" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" style="6" customWidth="1"/>
     <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="8"/>
   </cols>
@@ -33380,8 +33383,11 @@
       <c r="K1" s="9" t="s">
         <v>2419</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="L1" s="24" t="s">
+        <v>2417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -33401,11 +33407,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L2" s="8">
-        <f>ABS(K2-I2)</f>
+        <f t="shared" ref="L2:L10" si="0">ABS(K2-I2)</f>
         <v>0.2541844342707652</v>
       </c>
     </row>
-    <row r="3" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -33425,11 +33431,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L3" s="8">
-        <f>ABS(K3-I3)</f>
+        <f t="shared" si="0"/>
         <v>0.16572400261608897</v>
       </c>
     </row>
-    <row r="4" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -33449,11 +33455,11 @@
         <v>0.18181818181818182</v>
       </c>
       <c r="L4" s="8">
-        <f>ABS(K4-I4)</f>
+        <f t="shared" si="0"/>
         <v>0.13157357750163506</v>
       </c>
     </row>
-    <row r="5" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -33473,11 +33479,11 @@
         <v>0.18181818181818182</v>
       </c>
       <c r="L5" s="8">
-        <f>ABS(K5-I5)</f>
+        <f t="shared" si="0"/>
         <v>9.7491170699803786E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -33497,11 +33503,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L6" s="8">
-        <f>ABS(K6-I6)</f>
+        <f t="shared" si="0"/>
         <v>8.3369522563767173E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -33521,11 +33527,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L7" s="8">
-        <f>ABS(K7-I7)</f>
+        <f t="shared" si="0"/>
         <v>8.2333551340745589E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -33545,11 +33551,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L8" s="8">
-        <f>ABS(K8-I8)</f>
+        <f t="shared" si="0"/>
         <v>7.640549378678875E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -33569,11 +33575,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L9" s="8">
-        <f>ABS(K9-I9)</f>
+        <f t="shared" si="0"/>
         <v>7.5829954218443435E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -33593,11 +33599,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L10" s="8">
-        <f>ABS(K10-I10)</f>
+        <f t="shared" si="0"/>
         <v>6.7887508175277958E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2378</v>
       </c>
@@ -33674,13 +33680,13 @@
         <v>25</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>937</v>
+        <v>670</v>
       </c>
       <c r="H14" s="5">
-        <v>28</v>
+        <v>843</v>
       </c>
       <c r="I14" s="7">
-        <v>3.2176511146862789E-3</v>
+        <v>9.6874281774304752E-2</v>
       </c>
       <c r="J14" s="5">
         <v>1</v>
@@ -33690,7 +33696,7 @@
       </c>
       <c r="L14" s="8">
         <f>ABS(K14-I14)</f>
-        <v>5.5605878297078429E-2</v>
+        <v>3.8050752362540047E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33698,13 +33704,13 @@
         <v>25</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>874</v>
+        <v>950</v>
       </c>
       <c r="H15" s="5">
-        <v>52</v>
+        <v>693</v>
       </c>
       <c r="I15" s="7">
-        <v>5.9756377844173755E-3</v>
+        <v>7.9636865088485401E-2</v>
       </c>
       <c r="J15" s="5">
         <v>1</v>
@@ -33714,7 +33720,7 @@
       </c>
       <c r="L15" s="8">
         <f>ABS(K15-I15)</f>
-        <v>5.2847891627347328E-2</v>
+        <v>2.0813335676720696E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33722,13 +33728,13 @@
         <v>25</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>886</v>
+        <v>691</v>
       </c>
       <c r="H16" s="5">
-        <v>55</v>
+        <v>429</v>
       </c>
       <c r="I16" s="7">
-        <v>6.3203861181337622E-3</v>
+        <v>4.9299011721443346E-2</v>
       </c>
       <c r="J16" s="5">
         <v>1</v>
@@ -33738,7 +33744,7 @@
       </c>
       <c r="L16" s="8">
         <f>ABS(K16-I16)</f>
-        <v>5.2503143293630941E-2</v>
+        <v>9.5245176903213588E-3</v>
       </c>
     </row>
     <row r="17" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33746,13 +33752,13 @@
         <v>25</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>875</v>
+        <v>1007</v>
       </c>
       <c r="H17" s="5">
-        <v>81</v>
+        <v>383</v>
       </c>
       <c r="I17" s="7">
-        <v>9.3082050103424508E-3</v>
+        <v>4.4012870604458743E-2</v>
       </c>
       <c r="J17" s="5">
         <v>1</v>
@@ -33762,7 +33768,7 @@
       </c>
       <c r="L17" s="8">
         <f>ABS(K17-I17)</f>
-        <v>4.9515324401422256E-2</v>
+        <v>1.4810658807305963E-2</v>
       </c>
     </row>
     <row r="18" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33770,13 +33776,13 @@
         <v>25</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>905</v>
+        <v>698</v>
       </c>
       <c r="H18" s="5">
-        <v>85</v>
+        <v>337</v>
       </c>
       <c r="I18" s="7">
-        <v>9.7678694552976331E-3</v>
+        <v>3.8726729487474146E-2</v>
       </c>
       <c r="J18" s="5">
         <v>1</v>
@@ -33786,7 +33792,7 @@
       </c>
       <c r="L18" s="8">
         <f>ABS(K18-I18)</f>
-        <v>4.9055659956467074E-2</v>
+        <v>2.0096799924290559E-2</v>
       </c>
     </row>
     <row r="19" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33794,13 +33800,13 @@
         <v>25</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>623</v>
+        <v>993</v>
       </c>
       <c r="H19" s="5">
-        <v>87</v>
+        <v>319</v>
       </c>
       <c r="I19" s="7">
-        <v>9.9977016777752243E-3</v>
+        <v>3.6658239485175818E-2</v>
       </c>
       <c r="J19" s="5">
         <v>1</v>
@@ -33810,7 +33816,7 @@
       </c>
       <c r="L19" s="8">
         <f>ABS(K19-I19)</f>
-        <v>4.8825827733989483E-2</v>
+        <v>2.2165289926588887E-2</v>
       </c>
     </row>
     <row r="20" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33818,13 +33824,13 @@
         <v>25</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>641</v>
+        <v>754</v>
       </c>
       <c r="H20" s="5">
-        <v>127</v>
+        <v>278</v>
       </c>
       <c r="I20" s="7">
-        <v>1.4594346127327051E-2</v>
+        <v>3.19466789243852E-2</v>
       </c>
       <c r="J20" s="5">
         <v>1</v>
@@ -33834,7 +33840,7 @@
       </c>
       <c r="L20" s="8">
         <f>ABS(K20-I20)</f>
-        <v>4.4229183284437652E-2</v>
+        <v>2.6876850487379506E-2</v>
       </c>
     </row>
     <row r="21" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33866,13 +33872,13 @@
         <v>25</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>670</v>
+        <v>641</v>
       </c>
       <c r="H22" s="5">
-        <v>843</v>
+        <v>127</v>
       </c>
       <c r="I22" s="7">
-        <v>9.6874281774304752E-2</v>
+        <v>1.4594346127327051E-2</v>
       </c>
       <c r="J22" s="5">
         <v>1</v>
@@ -33882,7 +33888,7 @@
       </c>
       <c r="L22" s="8">
         <f>ABS(K22-I22)</f>
-        <v>3.8050752362540047E-2</v>
+        <v>4.4229183284437652E-2</v>
       </c>
     </row>
     <row r="23" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33890,13 +33896,13 @@
         <v>25</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>754</v>
+        <v>623</v>
       </c>
       <c r="H23" s="5">
-        <v>278</v>
+        <v>87</v>
       </c>
       <c r="I23" s="7">
-        <v>3.19466789243852E-2</v>
+        <v>9.9977016777752243E-3</v>
       </c>
       <c r="J23" s="5">
         <v>1</v>
@@ -33906,7 +33912,7 @@
       </c>
       <c r="L23" s="8">
         <f>ABS(K23-I23)</f>
-        <v>2.6876850487379506E-2</v>
+        <v>4.8825827733989483E-2</v>
       </c>
     </row>
     <row r="24" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33914,13 +33920,13 @@
         <v>25</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>993</v>
+        <v>905</v>
       </c>
       <c r="H24" s="5">
-        <v>319</v>
+        <v>85</v>
       </c>
       <c r="I24" s="7">
-        <v>3.6658239485175818E-2</v>
+        <v>9.7678694552976331E-3</v>
       </c>
       <c r="J24" s="5">
         <v>1</v>
@@ -33930,7 +33936,7 @@
       </c>
       <c r="L24" s="8">
         <f>ABS(K24-I24)</f>
-        <v>2.2165289926588887E-2</v>
+        <v>4.9055659956467074E-2</v>
       </c>
     </row>
     <row r="25" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33938,13 +33944,13 @@
         <v>25</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>950</v>
+        <v>875</v>
       </c>
       <c r="H25" s="5">
-        <v>693</v>
+        <v>81</v>
       </c>
       <c r="I25" s="7">
-        <v>7.9636865088485401E-2</v>
+        <v>9.3082050103424508E-3</v>
       </c>
       <c r="J25" s="5">
         <v>1</v>
@@ -33954,7 +33960,7 @@
       </c>
       <c r="L25" s="8">
         <f>ABS(K25-I25)</f>
-        <v>2.0813335676720696E-2</v>
+        <v>4.9515324401422256E-2</v>
       </c>
     </row>
     <row r="26" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33962,13 +33968,13 @@
         <v>25</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>698</v>
+        <v>886</v>
       </c>
       <c r="H26" s="5">
-        <v>337</v>
+        <v>55</v>
       </c>
       <c r="I26" s="7">
-        <v>3.8726729487474146E-2</v>
+        <v>6.3203861181337622E-3</v>
       </c>
       <c r="J26" s="5">
         <v>1</v>
@@ -33978,7 +33984,7 @@
       </c>
       <c r="L26" s="8">
         <f>ABS(K26-I26)</f>
-        <v>2.0096799924290559E-2</v>
+        <v>5.2503143293630941E-2</v>
       </c>
     </row>
     <row r="27" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -33986,13 +33992,13 @@
         <v>25</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>1007</v>
+        <v>874</v>
       </c>
       <c r="H27" s="5">
-        <v>383</v>
+        <v>52</v>
       </c>
       <c r="I27" s="7">
-        <v>4.4012870604458743E-2</v>
+        <v>5.9756377844173755E-3</v>
       </c>
       <c r="J27" s="5">
         <v>1</v>
@@ -34002,7 +34008,7 @@
       </c>
       <c r="L27" s="8">
         <f>ABS(K27-I27)</f>
-        <v>1.4810658807305963E-2</v>
+        <v>5.2847891627347328E-2</v>
       </c>
     </row>
     <row r="28" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -34010,13 +34016,13 @@
         <v>25</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>691</v>
+        <v>937</v>
       </c>
       <c r="H28" s="5">
-        <v>429</v>
+        <v>28</v>
       </c>
       <c r="I28" s="7">
-        <v>4.9299011721443346E-2</v>
+        <v>3.2176511146862789E-3</v>
       </c>
       <c r="J28" s="5">
         <v>1</v>
@@ -34026,7 +34032,7 @@
       </c>
       <c r="L28" s="8">
         <f>ABS(K28-I28)</f>
-        <v>9.5245176903213588E-3</v>
+        <v>5.5605878297078429E-2</v>
       </c>
     </row>
     <row r="29" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -34073,7 +34079,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="8">
-        <f t="shared" ref="L30:L60" si="0">ABS(K30-I30)</f>
+        <f t="shared" ref="L30:L60" si="1">ABS(K30-I30)</f>
         <v>0</v>
       </c>
     </row>
@@ -34255,14 +34261,14 @@
       <c r="B38" s="16"/>
       <c r="C38" s="17"/>
       <c r="D38" s="16"/>
-      <c r="G38" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="H38" s="5">
-        <v>217</v>
+      <c r="G38" s="22" t="s">
+        <v>420</v>
+      </c>
+      <c r="H38" s="23">
+        <v>1179</v>
       </c>
       <c r="I38" s="7">
-        <v>4.5751633986928102E-2</v>
+        <v>0.24857685009487665</v>
       </c>
       <c r="J38" s="5">
         <v>1</v>
@@ -34272,7 +34278,7 @@
       </c>
       <c r="L38" s="8">
         <f>ABS(K38-I38)</f>
-        <v>0.20424836601307189</v>
+        <v>1.4231499051233498E-3</v>
       </c>
     </row>
     <row r="39" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -34309,14 +34315,14 @@
       <c r="B40" s="16"/>
       <c r="C40" s="17"/>
       <c r="D40" s="16"/>
-      <c r="G40" s="22" t="s">
-        <v>420</v>
-      </c>
-      <c r="H40" s="23">
-        <v>1179</v>
+      <c r="G40" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="H40" s="5">
+        <v>217</v>
       </c>
       <c r="I40" s="7">
-        <v>0.24857685009487665</v>
+        <v>4.5751633986928102E-2</v>
       </c>
       <c r="J40" s="5">
         <v>1</v>
@@ -34326,7 +34332,7 @@
       </c>
       <c r="L40" s="8">
         <f>ABS(K40-I40)</f>
-        <v>1.4231499051233498E-3</v>
+        <v>0.20424836601307189</v>
       </c>
     </row>
     <row r="41" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -34361,23 +34367,23 @@
       <c r="C42" s="17"/>
       <c r="D42" s="16"/>
       <c r="G42" s="3" t="s">
-        <v>779</v>
+        <v>723</v>
       </c>
       <c r="H42" s="5">
-        <v>767</v>
+        <v>1883</v>
       </c>
       <c r="I42" s="7">
-        <v>0.19203805708562843</v>
+        <v>0.47145718577866802</v>
       </c>
       <c r="J42" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K42" s="8">
-        <v>9.0909090909090912E-2</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="L42" s="8">
         <f>ABS(K42-I42)</f>
-        <v>0.10112896617653752</v>
+        <v>1.6911731233213489E-2</v>
       </c>
     </row>
     <row r="43" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -34388,13 +34394,13 @@
       <c r="C43" s="17"/>
       <c r="D43" s="16"/>
       <c r="G43" s="3" t="s">
-        <v>944</v>
+        <v>779</v>
       </c>
       <c r="H43" s="5">
-        <v>93</v>
+        <v>767</v>
       </c>
       <c r="I43" s="7">
-        <v>2.3284927391086629E-2</v>
+        <v>0.19203805708562843</v>
       </c>
       <c r="J43" s="5">
         <v>1</v>
@@ -34404,7 +34410,7 @@
       </c>
       <c r="L43" s="8">
         <f>ABS(K43-I43)</f>
-        <v>6.7624163518004279E-2</v>
+        <v>0.10112896617653752</v>
       </c>
     </row>
     <row r="44" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -34442,13 +34448,13 @@
       <c r="C45" s="17"/>
       <c r="D45" s="16"/>
       <c r="G45" s="3" t="s">
-        <v>887</v>
+        <v>1009</v>
       </c>
       <c r="H45" s="5">
-        <v>153</v>
+        <v>303</v>
       </c>
       <c r="I45" s="7">
-        <v>3.8307461191787684E-2</v>
+        <v>7.5863795693540306E-2</v>
       </c>
       <c r="J45" s="5">
         <v>1</v>
@@ -34458,7 +34464,7 @@
       </c>
       <c r="L45" s="8">
         <f>ABS(K45-I45)</f>
-        <v>5.2601629717303228E-2</v>
+        <v>1.5045295215550605E-2</v>
       </c>
     </row>
     <row r="46" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -34496,23 +34502,23 @@
       <c r="C47" s="17"/>
       <c r="D47" s="16"/>
       <c r="G47" s="3" t="s">
-        <v>723</v>
+        <v>887</v>
       </c>
       <c r="H47" s="5">
-        <v>1883</v>
+        <v>153</v>
       </c>
       <c r="I47" s="7">
-        <v>0.47145718577866802</v>
+        <v>3.8307461191787684E-2</v>
       </c>
       <c r="J47" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K47" s="8">
-        <v>0.45454545454545453</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="L47" s="8">
         <f>ABS(K47-I47)</f>
-        <v>1.6911731233213489E-2</v>
+        <v>5.2601629717303228E-2</v>
       </c>
     </row>
     <row r="48" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -34523,13 +34529,13 @@
       <c r="C48" s="17"/>
       <c r="D48" s="16"/>
       <c r="G48" s="3" t="s">
-        <v>1009</v>
+        <v>944</v>
       </c>
       <c r="H48" s="5">
-        <v>303</v>
+        <v>93</v>
       </c>
       <c r="I48" s="7">
-        <v>7.5863795693540306E-2</v>
+        <v>2.3284927391086629E-2</v>
       </c>
       <c r="J48" s="5">
         <v>1</v>
@@ -34539,7 +34545,7 @@
       </c>
       <c r="L48" s="8">
         <f>ABS(K48-I48)</f>
-        <v>1.5045295215550605E-2</v>
+        <v>6.7624163518004279E-2</v>
       </c>
     </row>
     <row r="49" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -34595,13 +34601,13 @@
         <v>26</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>864</v>
+        <v>632</v>
       </c>
       <c r="H51" s="5">
-        <v>1091</v>
+        <v>4662</v>
       </c>
       <c r="I51" s="7">
-        <v>1.3620134328730868E-2</v>
+        <v>5.8200793987665728E-2</v>
       </c>
       <c r="J51" s="5">
         <v>1</v>
@@ -34611,7 +34617,7 @@
       </c>
       <c r="L51" s="8">
         <f>ABS(K51-I51)</f>
-        <v>0.1530465323379358</v>
+        <v>0.10846587267900093</v>
       </c>
     </row>
     <row r="52" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -34619,13 +34625,13 @@
         <v>26</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>807</v>
+        <v>769</v>
       </c>
       <c r="H52" s="5">
-        <v>1233</v>
+        <v>3961</v>
       </c>
       <c r="I52" s="7">
-        <v>1.5392874085540935E-2</v>
+        <v>4.9449451948765322E-2</v>
       </c>
       <c r="J52" s="5">
         <v>1</v>
@@ -34635,7 +34641,7 @@
       </c>
       <c r="L52" s="8">
         <f>ABS(K52-I52)</f>
-        <v>0.15127379258112572</v>
+        <v>0.11721721471790134</v>
       </c>
     </row>
     <row r="53" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -34667,13 +34673,13 @@
         <v>26</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>769</v>
+        <v>807</v>
       </c>
       <c r="H54" s="5">
-        <v>3961</v>
+        <v>1233</v>
       </c>
       <c r="I54" s="7">
-        <v>4.9449451948765322E-2</v>
+        <v>1.5392874085540935E-2</v>
       </c>
       <c r="J54" s="5">
         <v>1</v>
@@ -34683,7 +34689,7 @@
       </c>
       <c r="L54" s="8">
         <f>ABS(K54-I54)</f>
-        <v>0.11721721471790134</v>
+        <v>0.15127379258112572</v>
       </c>
     </row>
     <row r="55" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -34691,13 +34697,13 @@
         <v>26</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>632</v>
+        <v>864</v>
       </c>
       <c r="H55" s="5">
-        <v>4662</v>
+        <v>1091</v>
       </c>
       <c r="I55" s="7">
-        <v>5.8200793987665728E-2</v>
+        <v>1.3620134328730868E-2</v>
       </c>
       <c r="J55" s="5">
         <v>1</v>
@@ -34707,7 +34713,7 @@
       </c>
       <c r="L55" s="8">
         <f>ABS(K55-I55)</f>
-        <v>0.10846587267900093</v>
+        <v>0.1530465323379358</v>
       </c>
     </row>
     <row r="56" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -34784,7 +34790,7 @@
         <v>0.5</v>
       </c>
       <c r="L58" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.25792610678252126</v>
       </c>
     </row>
@@ -34835,7 +34841,7 @@
         <v>1</v>
       </c>
       <c r="L60" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -34897,14 +34903,14 @@
       <c r="B63" s="18"/>
       <c r="C63" s="19"/>
       <c r="D63" s="18"/>
-      <c r="G63" s="22" t="s">
-        <v>433</v>
-      </c>
-      <c r="H63" s="23">
-        <v>1325</v>
+      <c r="G63" s="3" t="s">
+        <v>817</v>
+      </c>
+      <c r="H63" s="5">
+        <v>244204</v>
       </c>
       <c r="I63" s="7">
-        <v>1.1974078154130335E-3</v>
+        <v>0.22068813445669766</v>
       </c>
       <c r="J63" s="5">
         <v>1</v>
@@ -34914,7 +34920,7 @@
       </c>
       <c r="L63" s="8">
         <f>ABS(K63-I63)</f>
-        <v>0.24880259218458697</v>
+        <v>2.931186554330234E-2</v>
       </c>
     </row>
     <row r="64" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -34951,14 +34957,14 @@
       <c r="B65" s="18"/>
       <c r="C65" s="19"/>
       <c r="D65" s="18"/>
-      <c r="G65" s="3" t="s">
-        <v>817</v>
-      </c>
-      <c r="H65" s="5">
-        <v>244204</v>
+      <c r="G65" s="22" t="s">
+        <v>433</v>
+      </c>
+      <c r="H65" s="23">
+        <v>1325</v>
       </c>
       <c r="I65" s="7">
-        <v>0.22068813445669766</v>
+        <v>1.1974078154130335E-3</v>
       </c>
       <c r="J65" s="5">
         <v>1</v>
@@ -34968,7 +34974,7 @@
       </c>
       <c r="L65" s="8">
         <f>ABS(K65-I65)</f>
-        <v>2.931186554330234E-2</v>
+        <v>0.24880259218458697</v>
       </c>
     </row>
     <row r="66" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -35018,7 +35024,7 @@
         <v>1</v>
       </c>
       <c r="L67" s="8">
-        <f t="shared" ref="L67" si="1">ABS(K67-I67)</f>
+        <f t="shared" ref="L67" si="2">ABS(K67-I67)</f>
         <v>0</v>
       </c>
     </row>
@@ -35066,7 +35072,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="L69" s="8">
-        <f>ABS(K69-I69)</f>
+        <f t="shared" ref="L69:L75" si="3">ABS(K69-I69)</f>
         <v>0.24685057935866345</v>
       </c>
     </row>
@@ -35090,7 +35096,7 @@
         <v>0.5</v>
       </c>
       <c r="L70" s="8">
-        <f>ABS(K70-I70)</f>
+        <f t="shared" si="3"/>
         <v>0.18552950687146319</v>
       </c>
     </row>
@@ -35114,7 +35120,7 @@
         <v>0.1875</v>
       </c>
       <c r="L71" s="8">
-        <f>ABS(K71-I71)</f>
+        <f t="shared" si="3"/>
         <v>0.16190043115063324</v>
       </c>
     </row>
@@ -35138,7 +35144,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="L72" s="8">
-        <f>ABS(K72-I72)</f>
+        <f t="shared" si="3"/>
         <v>0.11463105182789904</v>
       </c>
     </row>
@@ -35162,7 +35168,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="L73" s="8">
-        <f>ABS(K73-I73)</f>
+        <f t="shared" si="3"/>
         <v>4.9565481002425221E-2</v>
       </c>
     </row>
@@ -35186,7 +35192,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="L74" s="8">
-        <f>ABS(K74-I74)</f>
+        <f t="shared" si="3"/>
         <v>3.9000044911524298E-2</v>
       </c>
     </row>
@@ -35210,7 +35216,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="L75" s="8">
-        <f>ABS(K75-I75)</f>
+        <f t="shared" si="3"/>
         <v>3.4862570735650772E-3</v>
       </c>
     </row>
@@ -35300,13 +35306,13 @@
       <c r="C79" s="17"/>
       <c r="D79" s="16"/>
       <c r="G79" s="3" t="s">
-        <v>622</v>
+        <v>704</v>
       </c>
       <c r="H79" s="5">
-        <v>128</v>
+        <v>1101</v>
       </c>
       <c r="I79" s="7">
-        <v>1.1027828034806583E-2</v>
+        <v>9.4856552080640991E-2</v>
       </c>
       <c r="J79" s="5">
         <v>1</v>
@@ -35316,7 +35322,7 @@
       </c>
       <c r="L79" s="8">
         <f>ABS(K79-I79)</f>
-        <v>6.040074339376484E-2</v>
+        <v>2.3427980652069566E-2</v>
       </c>
     </row>
     <row r="80" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35327,13 +35333,13 @@
       <c r="C80" s="17"/>
       <c r="D80" s="16"/>
       <c r="G80" s="3" t="s">
-        <v>801</v>
+        <v>676</v>
       </c>
       <c r="H80" s="5">
-        <v>179</v>
+        <v>644</v>
       </c>
       <c r="I80" s="7">
-        <v>1.542172826742483E-2</v>
+        <v>5.5483759800120616E-2</v>
       </c>
       <c r="J80" s="5">
         <v>1</v>
@@ -35343,7 +35349,7 @@
       </c>
       <c r="L80" s="8">
         <f>ABS(K80-I80)</f>
-        <v>5.6006843161146597E-2</v>
+        <v>1.5944811628450808E-2</v>
       </c>
     </row>
     <row r="81" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35354,13 +35360,13 @@
       <c r="C81" s="17"/>
       <c r="D81" s="16"/>
       <c r="G81" s="3" t="s">
-        <v>752</v>
+        <v>877</v>
       </c>
       <c r="H81" s="5">
-        <v>181</v>
+        <v>479</v>
       </c>
       <c r="I81" s="7">
-        <v>1.5594038080468683E-2</v>
+        <v>4.1268200224002759E-2</v>
       </c>
       <c r="J81" s="5">
         <v>1</v>
@@ -35370,7 +35376,7 @@
       </c>
       <c r="L81" s="8">
         <f>ABS(K81-I81)</f>
-        <v>5.583453334810274E-2</v>
+        <v>3.0160371204568666E-2</v>
       </c>
     </row>
     <row r="82" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35381,13 +35387,13 @@
       <c r="C82" s="17"/>
       <c r="D82" s="16"/>
       <c r="G82" s="3" t="s">
-        <v>631</v>
+        <v>742</v>
       </c>
       <c r="H82" s="5">
-        <v>193</v>
+        <v>440</v>
       </c>
       <c r="I82" s="7">
-        <v>1.6627896958731798E-2</v>
+        <v>3.7908158869647629E-2</v>
       </c>
       <c r="J82" s="5">
         <v>1</v>
@@ -35397,7 +35403,7 @@
       </c>
       <c r="L82" s="8">
         <f>ABS(K82-I82)</f>
-        <v>5.4800674469839626E-2</v>
+        <v>3.3520412558923796E-2</v>
       </c>
     </row>
     <row r="83" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35408,13 +35414,13 @@
       <c r="C83" s="17"/>
       <c r="D83" s="16"/>
       <c r="G83" s="3" t="s">
-        <v>815</v>
+        <v>780</v>
       </c>
       <c r="H83" s="5">
-        <v>208</v>
+        <v>309</v>
       </c>
       <c r="I83" s="7">
-        <v>1.7920220556560697E-2</v>
+        <v>2.6621866115275266E-2</v>
       </c>
       <c r="J83" s="5">
         <v>1</v>
@@ -35424,7 +35430,7 @@
       </c>
       <c r="L83" s="8">
         <f>ABS(K83-I83)</f>
-        <v>5.3508350872010724E-2</v>
+        <v>4.4806705313296155E-2</v>
       </c>
     </row>
     <row r="84" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35435,13 +35441,13 @@
       <c r="C84" s="17"/>
       <c r="D84" s="16"/>
       <c r="G84" s="3" t="s">
-        <v>721</v>
+        <v>738</v>
       </c>
       <c r="H84" s="5">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="I84" s="7">
-        <v>2.3778754200051693E-2</v>
+        <v>2.429568363918325E-2</v>
       </c>
       <c r="J84" s="5">
         <v>1</v>
@@ -35451,7 +35457,7 @@
       </c>
       <c r="L84" s="8">
         <f>ABS(K84-I84)</f>
-        <v>4.7649817228519728E-2</v>
+        <v>4.7132887789388178E-2</v>
       </c>
     </row>
     <row r="85" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35462,13 +35468,13 @@
       <c r="C85" s="17"/>
       <c r="D85" s="16"/>
       <c r="G85" s="3" t="s">
-        <v>738</v>
+        <v>721</v>
       </c>
       <c r="H85" s="5">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="I85" s="7">
-        <v>2.429568363918325E-2</v>
+        <v>2.3778754200051693E-2</v>
       </c>
       <c r="J85" s="5">
         <v>1</v>
@@ -35478,7 +35484,7 @@
       </c>
       <c r="L85" s="8">
         <f>ABS(K85-I85)</f>
-        <v>4.7132887789388178E-2</v>
+        <v>4.7649817228519728E-2</v>
       </c>
     </row>
     <row r="86" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35489,13 +35495,13 @@
       <c r="C86" s="17"/>
       <c r="D86" s="16"/>
       <c r="G86" s="3" t="s">
-        <v>780</v>
+        <v>815</v>
       </c>
       <c r="H86" s="5">
-        <v>309</v>
+        <v>208</v>
       </c>
       <c r="I86" s="7">
-        <v>2.6621866115275266E-2</v>
+        <v>1.7920220556560697E-2</v>
       </c>
       <c r="J86" s="5">
         <v>1</v>
@@ -35505,7 +35511,7 @@
       </c>
       <c r="L86" s="8">
         <f>ABS(K86-I86)</f>
-        <v>4.4806705313296155E-2</v>
+        <v>5.3508350872010724E-2</v>
       </c>
     </row>
     <row r="87" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35516,13 +35522,13 @@
       <c r="C87" s="17"/>
       <c r="D87" s="16"/>
       <c r="G87" s="3" t="s">
-        <v>742</v>
+        <v>631</v>
       </c>
       <c r="H87" s="5">
-        <v>440</v>
+        <v>193</v>
       </c>
       <c r="I87" s="7">
-        <v>3.7908158869647629E-2</v>
+        <v>1.6627896958731798E-2</v>
       </c>
       <c r="J87" s="5">
         <v>1</v>
@@ -35532,7 +35538,7 @@
       </c>
       <c r="L87" s="8">
         <f>ABS(K87-I87)</f>
-        <v>3.3520412558923796E-2</v>
+        <v>5.4800674469839626E-2</v>
       </c>
     </row>
     <row r="88" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35543,13 +35549,13 @@
       <c r="C88" s="17"/>
       <c r="D88" s="16"/>
       <c r="G88" s="3" t="s">
-        <v>877</v>
+        <v>752</v>
       </c>
       <c r="H88" s="5">
-        <v>479</v>
+        <v>181</v>
       </c>
       <c r="I88" s="7">
-        <v>4.1268200224002759E-2</v>
+        <v>1.5594038080468683E-2</v>
       </c>
       <c r="J88" s="5">
         <v>1</v>
@@ -35559,7 +35565,7 @@
       </c>
       <c r="L88" s="8">
         <f>ABS(K88-I88)</f>
-        <v>3.0160371204568666E-2</v>
+        <v>5.583453334810274E-2</v>
       </c>
     </row>
     <row r="89" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35570,13 +35576,13 @@
       <c r="C89" s="17"/>
       <c r="D89" s="16"/>
       <c r="G89" s="3" t="s">
-        <v>704</v>
+        <v>801</v>
       </c>
       <c r="H89" s="5">
-        <v>1101</v>
+        <v>179</v>
       </c>
       <c r="I89" s="7">
-        <v>9.4856552080640991E-2</v>
+        <v>1.542172826742483E-2</v>
       </c>
       <c r="J89" s="5">
         <v>1</v>
@@ -35586,7 +35592,7 @@
       </c>
       <c r="L89" s="8">
         <f>ABS(K89-I89)</f>
-        <v>2.3427980652069566E-2</v>
+        <v>5.6006843161146597E-2</v>
       </c>
     </row>
     <row r="90" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35597,13 +35603,13 @@
       <c r="C90" s="17"/>
       <c r="D90" s="16"/>
       <c r="G90" s="3" t="s">
-        <v>676</v>
+        <v>622</v>
       </c>
       <c r="H90" s="5">
-        <v>644</v>
+        <v>128</v>
       </c>
       <c r="I90" s="7">
-        <v>5.5483759800120616E-2</v>
+        <v>1.1027828034806583E-2</v>
       </c>
       <c r="J90" s="5">
         <v>1</v>
@@ -35613,7 +35619,7 @@
       </c>
       <c r="L90" s="8">
         <f>ABS(K90-I90)</f>
-        <v>1.5944811628450808E-2</v>
+        <v>6.040074339376484E-2</v>
       </c>
     </row>
     <row r="91" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -35702,23 +35708,23 @@
       <c r="C94" s="17"/>
       <c r="D94" s="16"/>
       <c r="G94" s="3" t="s">
-        <v>980</v>
+        <v>897</v>
       </c>
       <c r="H94" s="5">
-        <v>3205</v>
+        <v>11184</v>
       </c>
       <c r="I94" s="7">
-        <v>4.4852776533811013E-2</v>
+        <v>0.15651589789520823</v>
       </c>
       <c r="J94" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K94" s="8">
-        <v>0.1111111111111111</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="L94" s="8">
         <f>ABS(K94-I94)</f>
-        <v>6.6258334577300099E-2</v>
+        <v>1.0150768771458429E-2</v>
       </c>
     </row>
     <row r="95" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35729,13 +35735,13 @@
       <c r="C95" s="17"/>
       <c r="D95" s="16"/>
       <c r="G95" s="3" t="s">
-        <v>979</v>
+        <v>609</v>
       </c>
       <c r="H95" s="5">
-        <v>199</v>
+        <v>7396</v>
       </c>
       <c r="I95" s="7">
-        <v>2.7849305866547245E-3</v>
+        <v>0.10350425436632334</v>
       </c>
       <c r="J95" s="5">
         <v>1</v>
@@ -35745,7 +35751,7 @@
       </c>
       <c r="L95" s="8">
         <f>ABS(K95-I95)</f>
-        <v>5.277062496890083E-2</v>
+        <v>4.7948698810767784E-2</v>
       </c>
     </row>
     <row r="96" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35755,14 +35761,14 @@
       <c r="B96" s="16"/>
       <c r="C96" s="17"/>
       <c r="D96" s="16"/>
-      <c r="G96" s="3" t="s">
-        <v>1015</v>
-      </c>
-      <c r="H96" s="5">
-        <v>476</v>
+      <c r="G96" s="22" t="s">
+        <v>453</v>
+      </c>
+      <c r="H96" s="23">
+        <v>4658</v>
       </c>
       <c r="I96" s="7">
-        <v>6.6614420062695925E-3</v>
+        <v>6.5186968204209578E-2</v>
       </c>
       <c r="J96" s="5">
         <v>1</v>
@@ -35772,7 +35778,7 @@
       </c>
       <c r="L96" s="8">
         <f>ABS(K96-I96)</f>
-        <v>4.889411354928596E-2</v>
+        <v>9.6314126486540252E-3</v>
       </c>
     </row>
     <row r="97" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35783,23 +35789,23 @@
       <c r="C97" s="17"/>
       <c r="D97" s="16"/>
       <c r="G97" s="3" t="s">
-        <v>609</v>
+        <v>980</v>
       </c>
       <c r="H97" s="5">
-        <v>7396</v>
+        <v>3205</v>
       </c>
       <c r="I97" s="7">
-        <v>0.10350425436632334</v>
+        <v>4.4852776533811013E-2</v>
       </c>
       <c r="J97" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K97" s="8">
-        <v>5.5555555555555552E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="L97" s="8">
         <f>ABS(K97-I97)</f>
-        <v>4.7948698810767784E-2</v>
+        <v>6.6258334577300099E-2</v>
       </c>
     </row>
     <row r="98" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35810,13 +35816,13 @@
       <c r="C98" s="17"/>
       <c r="D98" s="16"/>
       <c r="G98" s="3" t="s">
-        <v>833</v>
+        <v>652</v>
       </c>
       <c r="H98" s="5">
-        <v>657</v>
+        <v>2470</v>
       </c>
       <c r="I98" s="7">
-        <v>9.1944693237796683E-3</v>
+        <v>3.4566726377071207E-2</v>
       </c>
       <c r="J98" s="5">
         <v>1</v>
@@ -35826,7 +35832,7 @@
       </c>
       <c r="L98" s="8">
         <f>ABS(K98-I98)</f>
-        <v>4.6361086231775886E-2</v>
+        <v>2.0988829178484346E-2</v>
       </c>
     </row>
     <row r="99" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35837,13 +35843,13 @@
       <c r="C99" s="17"/>
       <c r="D99" s="16"/>
       <c r="G99" s="3" t="s">
-        <v>926</v>
+        <v>645</v>
       </c>
       <c r="H99" s="5">
-        <v>997</v>
+        <v>2085</v>
       </c>
       <c r="I99" s="7">
-        <v>1.3952642185400805E-2</v>
+        <v>2.9178795342588448E-2</v>
       </c>
       <c r="J99" s="5">
         <v>1</v>
@@ -35853,7 +35859,7 @@
       </c>
       <c r="L99" s="8">
         <f>ABS(K99-I99)</f>
-        <v>4.1602913370154745E-2</v>
+        <v>2.6376760212967105E-2</v>
       </c>
     </row>
     <row r="100" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35891,13 +35897,13 @@
       <c r="C101" s="17"/>
       <c r="D101" s="16"/>
       <c r="G101" s="3" t="s">
-        <v>645</v>
+        <v>926</v>
       </c>
       <c r="H101" s="5">
-        <v>2085</v>
+        <v>997</v>
       </c>
       <c r="I101" s="7">
-        <v>2.9178795342588448E-2</v>
+        <v>1.3952642185400805E-2</v>
       </c>
       <c r="J101" s="5">
         <v>1</v>
@@ -35907,7 +35913,7 @@
       </c>
       <c r="L101" s="8">
         <f>ABS(K101-I101)</f>
-        <v>2.6376760212967105E-2</v>
+        <v>4.1602913370154745E-2</v>
       </c>
     </row>
     <row r="102" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35918,13 +35924,13 @@
       <c r="C102" s="17"/>
       <c r="D102" s="16"/>
       <c r="G102" s="3" t="s">
-        <v>652</v>
+        <v>833</v>
       </c>
       <c r="H102" s="5">
-        <v>2470</v>
+        <v>657</v>
       </c>
       <c r="I102" s="7">
-        <v>3.4566726377071207E-2</v>
+        <v>9.1944693237796683E-3</v>
       </c>
       <c r="J102" s="5">
         <v>1</v>
@@ -35934,7 +35940,7 @@
       </c>
       <c r="L102" s="8">
         <f>ABS(K102-I102)</f>
-        <v>2.0988829178484346E-2</v>
+        <v>4.6361086231775886E-2</v>
       </c>
     </row>
     <row r="103" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35945,23 +35951,23 @@
       <c r="C103" s="17"/>
       <c r="D103" s="16"/>
       <c r="G103" s="3" t="s">
-        <v>897</v>
+        <v>1015</v>
       </c>
       <c r="H103" s="5">
-        <v>11184</v>
+        <v>476</v>
       </c>
       <c r="I103" s="7">
-        <v>0.15651589789520823</v>
+        <v>6.6614420062695925E-3</v>
       </c>
       <c r="J103" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K103" s="8">
-        <v>0.16666666666666666</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="L103" s="8">
         <f>ABS(K103-I103)</f>
-        <v>1.0150768771458429E-2</v>
+        <v>4.889411354928596E-2</v>
       </c>
     </row>
     <row r="104" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -35971,14 +35977,14 @@
       <c r="B104" s="16"/>
       <c r="C104" s="17"/>
       <c r="D104" s="16"/>
-      <c r="G104" s="22" t="s">
-        <v>453</v>
-      </c>
-      <c r="H104" s="23">
-        <v>4658</v>
+      <c r="G104" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="H104" s="5">
+        <v>199</v>
       </c>
       <c r="I104" s="7">
-        <v>6.5186968204209578E-2</v>
+        <v>2.7849305866547245E-3</v>
       </c>
       <c r="J104" s="5">
         <v>1</v>
@@ -35988,7 +35994,7 @@
       </c>
       <c r="L104" s="8">
         <f>ABS(K104-I104)</f>
-        <v>9.6314126486540252E-3</v>
+        <v>5.277062496890083E-2</v>
       </c>
     </row>
     <row r="105" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -36092,13 +36098,13 @@
         <v>18</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>942</v>
+        <v>751</v>
       </c>
       <c r="H109" s="5">
-        <v>1</v>
+        <v>3338</v>
       </c>
       <c r="I109" s="7">
-        <v>7.5665859564164649E-6</v>
+        <v>2.5257263922518161E-2</v>
       </c>
       <c r="J109" s="5">
         <v>1</v>
@@ -36108,7 +36114,7 @@
       </c>
       <c r="L109" s="8">
         <f>ABS(K109-I109)</f>
-        <v>2.0825766747376916E-2</v>
+        <v>4.4239305891848289E-3</v>
       </c>
     </row>
     <row r="110" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36116,13 +36122,13 @@
         <v>18</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>935</v>
+        <v>906</v>
       </c>
       <c r="H110" s="5">
-        <v>5</v>
+        <v>3158</v>
       </c>
       <c r="I110" s="7">
-        <v>3.7832929782082326E-5</v>
+        <v>2.3895278450363197E-2</v>
       </c>
       <c r="J110" s="5">
         <v>1</v>
@@ -36132,7 +36138,7 @@
       </c>
       <c r="L110" s="8">
         <f>ABS(K110-I110)</f>
-        <v>2.0795500403551249E-2</v>
+        <v>3.0619451170298649E-3</v>
       </c>
     </row>
     <row r="111" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36140,13 +36146,13 @@
         <v>18</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>649</v>
+        <v>955</v>
       </c>
       <c r="H111" s="5">
-        <v>12</v>
+        <v>2840</v>
       </c>
       <c r="I111" s="7">
-        <v>9.0799031476997572E-5</v>
+        <v>2.1489104116222759E-2</v>
       </c>
       <c r="J111" s="5">
         <v>1</v>
@@ -36156,7 +36162,7 @@
       </c>
       <c r="L111" s="8">
         <f>ABS(K111-I111)</f>
-        <v>2.0742534301856335E-2</v>
+        <v>6.5577078288942686E-4</v>
       </c>
     </row>
     <row r="112" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36164,13 +36170,13 @@
         <v>18</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>673</v>
+        <v>814</v>
       </c>
       <c r="H112" s="5">
-        <v>15</v>
+        <v>2258</v>
       </c>
       <c r="I112" s="7">
-        <v>1.1349878934624698E-4</v>
+        <v>1.7085351089588377E-2</v>
       </c>
       <c r="J112" s="5">
         <v>1</v>
@@ -36180,7 +36186,7 @@
       </c>
       <c r="L112" s="8">
         <f>ABS(K112-I112)</f>
-        <v>2.0719834543987084E-2</v>
+        <v>3.7479822437449552E-3</v>
       </c>
     </row>
     <row r="113" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36188,13 +36194,13 @@
         <v>18</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>662</v>
+        <v>974</v>
       </c>
       <c r="H113" s="5">
-        <v>22</v>
+        <v>2251</v>
       </c>
       <c r="I113" s="7">
-        <v>1.6646489104116222E-4</v>
+        <v>1.7032384987893463E-2</v>
       </c>
       <c r="J113" s="5">
         <v>1</v>
@@ -36204,7 +36210,7 @@
       </c>
       <c r="L113" s="8">
         <f>ABS(K113-I113)</f>
-        <v>2.066686844229217E-2</v>
+        <v>3.8009483454398696E-3</v>
       </c>
     </row>
     <row r="114" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36212,13 +36218,13 @@
         <v>18</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>834</v>
+        <v>607</v>
       </c>
       <c r="H114" s="5">
-        <v>35</v>
+        <v>2092</v>
       </c>
       <c r="I114" s="7">
-        <v>2.6483050847457627E-4</v>
+        <v>1.5829297820823245E-2</v>
       </c>
       <c r="J114" s="5">
         <v>1</v>
@@ -36228,7 +36234,7 @@
       </c>
       <c r="L114" s="8">
         <f>ABS(K114-I114)</f>
-        <v>2.0568502824858757E-2</v>
+        <v>5.0040355125100869E-3</v>
       </c>
     </row>
     <row r="115" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36236,13 +36242,13 @@
         <v>18</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>714</v>
+        <v>791</v>
       </c>
       <c r="H115" s="5">
-        <v>40</v>
+        <v>2014</v>
       </c>
       <c r="I115" s="7">
-        <v>3.0266343825665861E-4</v>
+        <v>1.523910411622276E-2</v>
       </c>
       <c r="J115" s="5">
         <v>1</v>
@@ -36252,7 +36258,7 @@
       </c>
       <c r="L115" s="8">
         <f>ABS(K115-I115)</f>
-        <v>2.0530669895076674E-2</v>
+        <v>5.5942292171105718E-3</v>
       </c>
     </row>
     <row r="116" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36260,13 +36266,13 @@
         <v>18</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>907</v>
+        <v>989</v>
       </c>
       <c r="H116" s="5">
-        <v>41</v>
+        <v>1953</v>
       </c>
       <c r="I116" s="7">
-        <v>3.1023002421307506E-4</v>
+        <v>1.4777542372881355E-2</v>
       </c>
       <c r="J116" s="5">
         <v>1</v>
@@ -36276,7 +36282,7 @@
       </c>
       <c r="L116" s="8">
         <f>ABS(K116-I116)</f>
-        <v>2.0523103309120258E-2</v>
+        <v>6.0557909604519768E-3</v>
       </c>
     </row>
     <row r="117" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36284,13 +36290,13 @@
         <v>18</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>715</v>
+        <v>933</v>
       </c>
       <c r="H117" s="5">
-        <v>45</v>
+        <v>1841</v>
       </c>
       <c r="I117" s="7">
-        <v>3.404963680387409E-4</v>
+        <v>1.3930084745762713E-2</v>
       </c>
       <c r="J117" s="5">
         <v>1</v>
@@ -36300,7 +36306,7 @@
       </c>
       <c r="L117" s="8">
         <f>ABS(K117-I117)</f>
-        <v>2.0492836965294591E-2</v>
+        <v>6.9032485875706196E-3</v>
       </c>
     </row>
     <row r="118" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36308,13 +36314,13 @@
         <v>18</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>850</v>
+        <v>967</v>
       </c>
       <c r="H118" s="5">
-        <v>45</v>
+        <v>1816</v>
       </c>
       <c r="I118" s="7">
-        <v>3.404963680387409E-4</v>
+        <v>1.3740920096852301E-2</v>
       </c>
       <c r="J118" s="5">
         <v>1</v>
@@ -36324,7 +36330,7 @@
       </c>
       <c r="L118" s="8">
         <f>ABS(K118-I118)</f>
-        <v>2.0492836965294591E-2</v>
+        <v>7.0924132364810315E-3</v>
       </c>
     </row>
     <row r="119" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36332,13 +36338,13 @@
         <v>18</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>867</v>
+        <v>915</v>
       </c>
       <c r="H119" s="5">
-        <v>53</v>
+        <v>1676</v>
       </c>
       <c r="I119" s="7">
-        <v>4.0102905569007263E-4</v>
+        <v>1.2681598062953995E-2</v>
       </c>
       <c r="J119" s="5">
         <v>1</v>
@@ -36348,7 +36354,7 @@
       </c>
       <c r="L119" s="8">
         <f>ABS(K119-I119)</f>
-        <v>2.0432304277643261E-2</v>
+        <v>8.1517352703793372E-3</v>
       </c>
     </row>
     <row r="120" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36356,13 +36362,13 @@
         <v>18</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>627</v>
+        <v>794</v>
       </c>
       <c r="H120" s="5">
-        <v>83</v>
+        <v>1254</v>
       </c>
       <c r="I120" s="7">
-        <v>6.2802663438256661E-4</v>
+        <v>9.4884987893462478E-3</v>
       </c>
       <c r="J120" s="5">
         <v>1</v>
@@ -36372,7 +36378,7 @@
       </c>
       <c r="L120" s="8">
         <f>ABS(K120-I120)</f>
-        <v>2.0205306698950765E-2</v>
+        <v>1.1344834543987084E-2</v>
       </c>
     </row>
     <row r="121" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36380,13 +36386,13 @@
         <v>18</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>932</v>
+        <v>987</v>
       </c>
       <c r="H121" s="5">
-        <v>134</v>
+        <v>981</v>
       </c>
       <c r="I121" s="7">
-        <v>1.0139225181598063E-3</v>
+        <v>7.4228208232445516E-3</v>
       </c>
       <c r="J121" s="5">
         <v>1</v>
@@ -36396,7 +36402,7 @@
       </c>
       <c r="L121" s="8">
         <f>ABS(K121-I121)</f>
-        <v>1.9819410815173525E-2</v>
+        <v>1.341051251008878E-2</v>
       </c>
     </row>
     <row r="122" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36404,13 +36410,13 @@
         <v>18</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>644</v>
+        <v>956</v>
       </c>
       <c r="H122" s="5">
-        <v>138</v>
+        <v>960</v>
       </c>
       <c r="I122" s="7">
-        <v>1.0441888619854721E-3</v>
+        <v>7.2639225181598066E-3</v>
       </c>
       <c r="J122" s="5">
         <v>1</v>
@@ -36420,7 +36426,7 @@
       </c>
       <c r="L122" s="8">
         <f>ABS(K122-I122)</f>
-        <v>1.9789144471347862E-2</v>
+        <v>1.3569410815173526E-2</v>
       </c>
     </row>
     <row r="123" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36428,13 +36434,13 @@
         <v>18</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>936</v>
+        <v>686</v>
       </c>
       <c r="H123" s="5">
-        <v>152</v>
+        <v>892</v>
       </c>
       <c r="I123" s="7">
-        <v>1.1501210653753027E-3</v>
+        <v>6.7493946731234863E-3</v>
       </c>
       <c r="J123" s="5">
         <v>1</v>
@@ -36444,7 +36450,7 @@
       </c>
       <c r="L123" s="8">
         <f>ABS(K123-I123)</f>
-        <v>1.9683212267958029E-2</v>
+        <v>1.4083938660209846E-2</v>
       </c>
     </row>
     <row r="124" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36452,13 +36458,13 @@
         <v>18</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>975</v>
+        <v>966</v>
       </c>
       <c r="H124" s="5">
-        <v>152</v>
+        <v>864</v>
       </c>
       <c r="I124" s="7">
-        <v>1.1501210653753027E-3</v>
+        <v>6.5375302663438261E-3</v>
       </c>
       <c r="J124" s="5">
         <v>1</v>
@@ -36468,7 +36474,7 @@
       </c>
       <c r="L124" s="8">
         <f>ABS(K124-I124)</f>
-        <v>1.9683212267958029E-2</v>
+        <v>1.4295803066989507E-2</v>
       </c>
     </row>
     <row r="125" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36476,13 +36482,13 @@
         <v>18</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>1005</v>
+        <v>943</v>
       </c>
       <c r="H125" s="5">
-        <v>180</v>
+        <v>829</v>
       </c>
       <c r="I125" s="7">
-        <v>1.3619854721549636E-3</v>
+        <v>6.2726997578692496E-3</v>
       </c>
       <c r="J125" s="5">
         <v>1</v>
@@ -36492,7 +36498,7 @@
       </c>
       <c r="L125" s="8">
         <f>ABS(K125-I125)</f>
-        <v>1.9471347861178368E-2</v>
+        <v>1.4560633575464083E-2</v>
       </c>
     </row>
     <row r="126" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36500,13 +36506,13 @@
         <v>18</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>1002</v>
+        <v>968</v>
       </c>
       <c r="H126" s="5">
-        <v>263</v>
+        <v>785</v>
       </c>
       <c r="I126" s="7">
-        <v>1.9900121065375303E-3</v>
+        <v>5.9397699757869253E-3</v>
       </c>
       <c r="J126" s="5">
         <v>1</v>
@@ -36516,7 +36522,7 @@
       </c>
       <c r="L126" s="8">
         <f>ABS(K126-I126)</f>
-        <v>1.8843321226795801E-2</v>
+        <v>1.4893563357546408E-2</v>
       </c>
     </row>
     <row r="127" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36524,13 +36530,13 @@
         <v>18</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>762</v>
+        <v>972</v>
       </c>
       <c r="H127" s="5">
-        <v>303</v>
+        <v>643</v>
       </c>
       <c r="I127" s="7">
-        <v>2.292675544794189E-3</v>
+        <v>4.865314769975787E-3</v>
       </c>
       <c r="J127" s="5">
         <v>1</v>
@@ -36540,7 +36546,7 @@
       </c>
       <c r="L127" s="8">
         <f>ABS(K127-I127)</f>
-        <v>1.8540657788539142E-2</v>
+        <v>1.5968018563357545E-2</v>
       </c>
     </row>
     <row r="128" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36548,13 +36554,13 @@
         <v>18</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>973</v>
+        <v>990</v>
       </c>
       <c r="H128" s="5">
-        <v>317</v>
+        <v>541</v>
       </c>
       <c r="I128" s="7">
-        <v>2.3986077481840192E-3</v>
+        <v>4.0935230024213079E-3</v>
       </c>
       <c r="J128" s="5">
         <v>1</v>
@@ -36564,7 +36570,7 @@
       </c>
       <c r="L128" s="8">
         <f>ABS(K128-I128)</f>
-        <v>1.8434725585149313E-2</v>
+        <v>1.6739810330912024E-2</v>
       </c>
     </row>
     <row r="129" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36572,13 +36578,13 @@
         <v>18</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>960</v>
+        <v>921</v>
       </c>
       <c r="H129" s="5">
-        <v>341</v>
+        <v>525</v>
       </c>
       <c r="I129" s="7">
-        <v>2.5802058111380147E-3</v>
+        <v>3.9724576271186439E-3</v>
       </c>
       <c r="J129" s="5">
         <v>1</v>
@@ -36588,7 +36594,7 @@
       </c>
       <c r="L129" s="8">
         <f>ABS(K129-I129)</f>
-        <v>1.8253127522195316E-2</v>
+        <v>1.6860875706214688E-2</v>
       </c>
     </row>
     <row r="130" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36596,13 +36602,13 @@
         <v>18</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>941</v>
+        <v>638</v>
       </c>
       <c r="H130" s="5">
-        <v>444</v>
+        <v>477</v>
       </c>
       <c r="I130" s="7">
-        <v>3.3595641646489106E-3</v>
+        <v>3.6092615012106536E-3</v>
       </c>
       <c r="J130" s="5">
         <v>1</v>
@@ -36612,7 +36618,7 @@
       </c>
       <c r="L130" s="8">
         <f>ABS(K130-I130)</f>
-        <v>1.7473769168684421E-2</v>
+        <v>1.7224071832122677E-2</v>
       </c>
     </row>
     <row r="131" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36644,13 +36650,13 @@
         <v>18</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>638</v>
+        <v>941</v>
       </c>
       <c r="H132" s="5">
-        <v>477</v>
+        <v>444</v>
       </c>
       <c r="I132" s="7">
-        <v>3.6092615012106536E-3</v>
+        <v>3.3595641646489106E-3</v>
       </c>
       <c r="J132" s="5">
         <v>1</v>
@@ -36660,7 +36666,7 @@
       </c>
       <c r="L132" s="8">
         <f>ABS(K132-I132)</f>
-        <v>1.7224071832122677E-2</v>
+        <v>1.7473769168684421E-2</v>
       </c>
     </row>
     <row r="133" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36668,13 +36674,13 @@
         <v>18</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>921</v>
+        <v>960</v>
       </c>
       <c r="H133" s="5">
-        <v>525</v>
+        <v>341</v>
       </c>
       <c r="I133" s="7">
-        <v>3.9724576271186439E-3</v>
+        <v>2.5802058111380147E-3</v>
       </c>
       <c r="J133" s="5">
         <v>1</v>
@@ -36684,7 +36690,7 @@
       </c>
       <c r="L133" s="8">
         <f>ABS(K133-I133)</f>
-        <v>1.6860875706214688E-2</v>
+        <v>1.8253127522195316E-2</v>
       </c>
     </row>
     <row r="134" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36692,13 +36698,13 @@
         <v>18</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>990</v>
+        <v>973</v>
       </c>
       <c r="H134" s="5">
-        <v>541</v>
+        <v>317</v>
       </c>
       <c r="I134" s="7">
-        <v>4.0935230024213079E-3</v>
+        <v>2.3986077481840192E-3</v>
       </c>
       <c r="J134" s="5">
         <v>1</v>
@@ -36708,7 +36714,7 @@
       </c>
       <c r="L134" s="8">
         <f>ABS(K134-I134)</f>
-        <v>1.6739810330912024E-2</v>
+        <v>1.8434725585149313E-2</v>
       </c>
     </row>
     <row r="135" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36716,13 +36722,13 @@
         <v>18</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>972</v>
+        <v>762</v>
       </c>
       <c r="H135" s="5">
-        <v>643</v>
+        <v>303</v>
       </c>
       <c r="I135" s="7">
-        <v>4.865314769975787E-3</v>
+        <v>2.292675544794189E-3</v>
       </c>
       <c r="J135" s="5">
         <v>1</v>
@@ -36732,7 +36738,7 @@
       </c>
       <c r="L135" s="8">
         <f>ABS(K135-I135)</f>
-        <v>1.5968018563357545E-2</v>
+        <v>1.8540657788539142E-2</v>
       </c>
     </row>
     <row r="136" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36740,13 +36746,13 @@
         <v>18</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>968</v>
+        <v>1002</v>
       </c>
       <c r="H136" s="5">
-        <v>785</v>
+        <v>263</v>
       </c>
       <c r="I136" s="7">
-        <v>5.9397699757869253E-3</v>
+        <v>1.9900121065375303E-3</v>
       </c>
       <c r="J136" s="5">
         <v>1</v>
@@ -36756,7 +36762,7 @@
       </c>
       <c r="L136" s="8">
         <f>ABS(K136-I136)</f>
-        <v>1.4893563357546408E-2</v>
+        <v>1.8843321226795801E-2</v>
       </c>
     </row>
     <row r="137" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36764,13 +36770,13 @@
         <v>18</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>943</v>
+        <v>1005</v>
       </c>
       <c r="H137" s="5">
-        <v>829</v>
+        <v>180</v>
       </c>
       <c r="I137" s="7">
-        <v>6.2726997578692496E-3</v>
+        <v>1.3619854721549636E-3</v>
       </c>
       <c r="J137" s="5">
         <v>1</v>
@@ -36780,7 +36786,7 @@
       </c>
       <c r="L137" s="8">
         <f>ABS(K137-I137)</f>
-        <v>1.4560633575464083E-2</v>
+        <v>1.9471347861178368E-2</v>
       </c>
     </row>
     <row r="138" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36788,13 +36794,13 @@
         <v>18</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>966</v>
+        <v>936</v>
       </c>
       <c r="H138" s="5">
-        <v>864</v>
+        <v>152</v>
       </c>
       <c r="I138" s="7">
-        <v>6.5375302663438261E-3</v>
+        <v>1.1501210653753027E-3</v>
       </c>
       <c r="J138" s="5">
         <v>1</v>
@@ -36804,7 +36810,7 @@
       </c>
       <c r="L138" s="8">
         <f>ABS(K138-I138)</f>
-        <v>1.4295803066989507E-2</v>
+        <v>1.9683212267958029E-2</v>
       </c>
     </row>
     <row r="139" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36812,13 +36818,13 @@
         <v>18</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>686</v>
+        <v>975</v>
       </c>
       <c r="H139" s="5">
-        <v>892</v>
+        <v>152</v>
       </c>
       <c r="I139" s="7">
-        <v>6.7493946731234863E-3</v>
+        <v>1.1501210653753027E-3</v>
       </c>
       <c r="J139" s="5">
         <v>1</v>
@@ -36828,7 +36834,7 @@
       </c>
       <c r="L139" s="8">
         <f>ABS(K139-I139)</f>
-        <v>1.4083938660209846E-2</v>
+        <v>1.9683212267958029E-2</v>
       </c>
     </row>
     <row r="140" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36836,13 +36842,13 @@
         <v>18</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>956</v>
+        <v>644</v>
       </c>
       <c r="H140" s="5">
-        <v>960</v>
+        <v>138</v>
       </c>
       <c r="I140" s="7">
-        <v>7.2639225181598066E-3</v>
+        <v>1.0441888619854721E-3</v>
       </c>
       <c r="J140" s="5">
         <v>1</v>
@@ -36852,7 +36858,7 @@
       </c>
       <c r="L140" s="8">
         <f>ABS(K140-I140)</f>
-        <v>1.3569410815173526E-2</v>
+        <v>1.9789144471347862E-2</v>
       </c>
     </row>
     <row r="141" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36860,13 +36866,13 @@
         <v>18</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>987</v>
+        <v>932</v>
       </c>
       <c r="H141" s="5">
-        <v>981</v>
+        <v>134</v>
       </c>
       <c r="I141" s="7">
-        <v>7.4228208232445516E-3</v>
+        <v>1.0139225181598063E-3</v>
       </c>
       <c r="J141" s="5">
         <v>1</v>
@@ -36876,7 +36882,7 @@
       </c>
       <c r="L141" s="8">
         <f>ABS(K141-I141)</f>
-        <v>1.341051251008878E-2</v>
+        <v>1.9819410815173525E-2</v>
       </c>
     </row>
     <row r="142" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36884,13 +36890,13 @@
         <v>18</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>794</v>
+        <v>627</v>
       </c>
       <c r="H142" s="5">
-        <v>1254</v>
+        <v>83</v>
       </c>
       <c r="I142" s="7">
-        <v>9.4884987893462478E-3</v>
+        <v>6.2802663438256661E-4</v>
       </c>
       <c r="J142" s="5">
         <v>1</v>
@@ -36900,7 +36906,7 @@
       </c>
       <c r="L142" s="8">
         <f>ABS(K142-I142)</f>
-        <v>1.1344834543987084E-2</v>
+        <v>2.0205306698950765E-2</v>
       </c>
     </row>
     <row r="143" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36908,13 +36914,13 @@
         <v>18</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>915</v>
+        <v>867</v>
       </c>
       <c r="H143" s="5">
-        <v>1676</v>
+        <v>53</v>
       </c>
       <c r="I143" s="7">
-        <v>1.2681598062953995E-2</v>
+        <v>4.0102905569007263E-4</v>
       </c>
       <c r="J143" s="5">
         <v>1</v>
@@ -36924,7 +36930,7 @@
       </c>
       <c r="L143" s="8">
         <f>ABS(K143-I143)</f>
-        <v>8.1517352703793372E-3</v>
+        <v>2.0432304277643261E-2</v>
       </c>
     </row>
     <row r="144" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36932,13 +36938,13 @@
         <v>18</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>967</v>
+        <v>715</v>
       </c>
       <c r="H144" s="5">
-        <v>1816</v>
+        <v>45</v>
       </c>
       <c r="I144" s="7">
-        <v>1.3740920096852301E-2</v>
+        <v>3.404963680387409E-4</v>
       </c>
       <c r="J144" s="5">
         <v>1</v>
@@ -36948,7 +36954,7 @@
       </c>
       <c r="L144" s="8">
         <f>ABS(K144-I144)</f>
-        <v>7.0924132364810315E-3</v>
+        <v>2.0492836965294591E-2</v>
       </c>
     </row>
     <row r="145" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36956,13 +36962,13 @@
         <v>18</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>933</v>
+        <v>850</v>
       </c>
       <c r="H145" s="5">
-        <v>1841</v>
+        <v>45</v>
       </c>
       <c r="I145" s="7">
-        <v>1.3930084745762713E-2</v>
+        <v>3.404963680387409E-4</v>
       </c>
       <c r="J145" s="5">
         <v>1</v>
@@ -36972,7 +36978,7 @@
       </c>
       <c r="L145" s="8">
         <f>ABS(K145-I145)</f>
-        <v>6.9032485875706196E-3</v>
+        <v>2.0492836965294591E-2</v>
       </c>
     </row>
     <row r="146" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -36980,13 +36986,13 @@
         <v>18</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>989</v>
+        <v>907</v>
       </c>
       <c r="H146" s="5">
-        <v>1953</v>
+        <v>41</v>
       </c>
       <c r="I146" s="7">
-        <v>1.4777542372881355E-2</v>
+        <v>3.1023002421307506E-4</v>
       </c>
       <c r="J146" s="5">
         <v>1</v>
@@ -36996,7 +37002,7 @@
       </c>
       <c r="L146" s="8">
         <f>ABS(K146-I146)</f>
-        <v>6.0557909604519768E-3</v>
+        <v>2.0523103309120258E-2</v>
       </c>
     </row>
     <row r="147" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37004,13 +37010,13 @@
         <v>18</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>791</v>
+        <v>714</v>
       </c>
       <c r="H147" s="5">
-        <v>2014</v>
+        <v>40</v>
       </c>
       <c r="I147" s="7">
-        <v>1.523910411622276E-2</v>
+        <v>3.0266343825665861E-4</v>
       </c>
       <c r="J147" s="5">
         <v>1</v>
@@ -37020,7 +37026,7 @@
       </c>
       <c r="L147" s="8">
         <f>ABS(K147-I147)</f>
-        <v>5.5942292171105718E-3</v>
+        <v>2.0530669895076674E-2</v>
       </c>
     </row>
     <row r="148" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37028,13 +37034,13 @@
         <v>18</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>607</v>
+        <v>834</v>
       </c>
       <c r="H148" s="5">
-        <v>2092</v>
+        <v>35</v>
       </c>
       <c r="I148" s="7">
-        <v>1.5829297820823245E-2</v>
+        <v>2.6483050847457627E-4</v>
       </c>
       <c r="J148" s="5">
         <v>1</v>
@@ -37044,7 +37050,7 @@
       </c>
       <c r="L148" s="8">
         <f>ABS(K148-I148)</f>
-        <v>5.0040355125100869E-3</v>
+        <v>2.0568502824858757E-2</v>
       </c>
     </row>
     <row r="149" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37052,13 +37058,13 @@
         <v>18</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>751</v>
+        <v>662</v>
       </c>
       <c r="H149" s="5">
-        <v>3338</v>
+        <v>22</v>
       </c>
       <c r="I149" s="7">
-        <v>2.5257263922518161E-2</v>
+        <v>1.6646489104116222E-4</v>
       </c>
       <c r="J149" s="5">
         <v>1</v>
@@ -37068,7 +37074,7 @@
       </c>
       <c r="L149" s="8">
         <f>ABS(K149-I149)</f>
-        <v>4.4239305891848289E-3</v>
+        <v>2.066686844229217E-2</v>
       </c>
     </row>
     <row r="150" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37076,13 +37082,13 @@
         <v>18</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>974</v>
+        <v>673</v>
       </c>
       <c r="H150" s="5">
-        <v>2251</v>
+        <v>15</v>
       </c>
       <c r="I150" s="7">
-        <v>1.7032384987893463E-2</v>
+        <v>1.1349878934624698E-4</v>
       </c>
       <c r="J150" s="5">
         <v>1</v>
@@ -37092,7 +37098,7 @@
       </c>
       <c r="L150" s="8">
         <f>ABS(K150-I150)</f>
-        <v>3.8009483454398696E-3</v>
+        <v>2.0719834543987084E-2</v>
       </c>
     </row>
     <row r="151" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37100,13 +37106,13 @@
         <v>18</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>814</v>
+        <v>649</v>
       </c>
       <c r="H151" s="5">
-        <v>2258</v>
+        <v>12</v>
       </c>
       <c r="I151" s="7">
-        <v>1.7085351089588377E-2</v>
+        <v>9.0799031476997572E-5</v>
       </c>
       <c r="J151" s="5">
         <v>1</v>
@@ -37116,7 +37122,7 @@
       </c>
       <c r="L151" s="8">
         <f>ABS(K151-I151)</f>
-        <v>3.7479822437449552E-3</v>
+        <v>2.0742534301856335E-2</v>
       </c>
     </row>
     <row r="152" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37124,13 +37130,13 @@
         <v>18</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>906</v>
+        <v>935</v>
       </c>
       <c r="H152" s="5">
-        <v>3158</v>
+        <v>5</v>
       </c>
       <c r="I152" s="7">
-        <v>2.3895278450363197E-2</v>
+        <v>3.7832929782082326E-5</v>
       </c>
       <c r="J152" s="5">
         <v>1</v>
@@ -37140,7 +37146,7 @@
       </c>
       <c r="L152" s="8">
         <f>ABS(K152-I152)</f>
-        <v>3.0619451170298649E-3</v>
+        <v>2.0795500403551249E-2</v>
       </c>
     </row>
     <row r="153" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37148,13 +37154,13 @@
         <v>18</v>
       </c>
       <c r="G153" s="3" t="s">
-        <v>955</v>
+        <v>942</v>
       </c>
       <c r="H153" s="5">
-        <v>2840</v>
+        <v>1</v>
       </c>
       <c r="I153" s="7">
-        <v>2.1489104116222759E-2</v>
+        <v>7.5665859564164649E-6</v>
       </c>
       <c r="J153" s="5">
         <v>1</v>
@@ -37164,7 +37170,7 @@
       </c>
       <c r="L153" s="8">
         <f>ABS(K153-I153)</f>
-        <v>6.5577078288942686E-4</v>
+        <v>2.0825766747376916E-2</v>
       </c>
     </row>
     <row r="154" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -37219,14 +37225,14 @@
       <c r="A156" t="s">
         <v>30</v>
       </c>
-      <c r="G156" s="3" t="s">
-        <v>893</v>
-      </c>
-      <c r="H156" s="5">
-        <v>328</v>
+      <c r="G156" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="H156" s="23">
+        <v>8376</v>
       </c>
       <c r="I156" s="7">
-        <v>4.4331513218359734E-3</v>
+        <v>0.11320754716981132</v>
       </c>
       <c r="J156" s="5">
         <v>1</v>
@@ -37236,7 +37242,7 @@
       </c>
       <c r="L156" s="8">
         <f>ABS(K156-I156)</f>
-        <v>0.13842399153530688</v>
+        <v>2.9649595687331526E-2</v>
       </c>
     </row>
     <row r="157" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37244,13 +37250,13 @@
         <v>30</v>
       </c>
       <c r="G157" s="3" t="s">
-        <v>664</v>
+        <v>650</v>
       </c>
       <c r="H157" s="5">
-        <v>632</v>
+        <v>8015</v>
       </c>
       <c r="I157" s="7">
-        <v>8.5419257176839493E-3</v>
+        <v>0.10832837757474185</v>
       </c>
       <c r="J157" s="5">
         <v>1</v>
@@ -37260,7 +37266,7 @@
       </c>
       <c r="L157" s="8">
         <f>ABS(K157-I157)</f>
-        <v>0.1343152171394589</v>
+        <v>3.4528765282400994E-2</v>
       </c>
     </row>
     <row r="158" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37268,13 +37274,13 @@
         <v>30</v>
       </c>
       <c r="G158" s="3" t="s">
-        <v>674</v>
+        <v>957</v>
       </c>
       <c r="H158" s="5">
-        <v>2620</v>
+        <v>4673</v>
       </c>
       <c r="I158" s="7">
-        <v>3.5411147753689788E-2</v>
+        <v>6.3158890630913123E-2</v>
       </c>
       <c r="J158" s="5">
         <v>1</v>
@@ -37284,7 +37290,7 @@
       </c>
       <c r="L158" s="8">
         <f>ABS(K158-I158)</f>
-        <v>0.10744599510345307</v>
+        <v>7.9698252226229727E-2</v>
       </c>
     </row>
     <row r="159" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37292,13 +37298,13 @@
         <v>30</v>
       </c>
       <c r="G159" s="3" t="s">
-        <v>957</v>
+        <v>674</v>
       </c>
       <c r="H159" s="5">
-        <v>4673</v>
+        <v>2620</v>
       </c>
       <c r="I159" s="7">
-        <v>6.3158890630913123E-2</v>
+        <v>3.5411147753689788E-2</v>
       </c>
       <c r="J159" s="5">
         <v>1</v>
@@ -37308,7 +37314,7 @@
       </c>
       <c r="L159" s="8">
         <f>ABS(K159-I159)</f>
-        <v>7.9698252226229727E-2</v>
+        <v>0.10744599510345307</v>
       </c>
     </row>
     <row r="160" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37316,13 +37322,13 @@
         <v>30</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>650</v>
+        <v>664</v>
       </c>
       <c r="H160" s="5">
-        <v>8015</v>
+        <v>632</v>
       </c>
       <c r="I160" s="7">
-        <v>0.10832837757474185</v>
+        <v>8.5419257176839493E-3</v>
       </c>
       <c r="J160" s="5">
         <v>1</v>
@@ -37332,21 +37338,21 @@
       </c>
       <c r="L160" s="8">
         <f>ABS(K160-I160)</f>
-        <v>3.4528765282400994E-2</v>
+        <v>0.1343152171394589</v>
       </c>
     </row>
     <row r="161" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>30</v>
       </c>
-      <c r="G161" s="22" t="s">
-        <v>459</v>
-      </c>
-      <c r="H161" s="23">
-        <v>8376</v>
+      <c r="G161" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="H161" s="5">
+        <v>328</v>
       </c>
       <c r="I161" s="7">
-        <v>0.11320754716981132</v>
+        <v>4.4331513218359734E-3</v>
       </c>
       <c r="J161" s="5">
         <v>1</v>
@@ -37356,7 +37362,7 @@
       </c>
       <c r="L161" s="8">
         <f>ABS(K161-I161)</f>
-        <v>2.9649595687331526E-2</v>
+        <v>0.13842399153530688</v>
       </c>
     </row>
     <row r="162" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -37406,7 +37412,7 @@
         <v>1</v>
       </c>
       <c r="L163" s="8">
-        <f t="shared" ref="L163:L194" si="2">ABS(K163-I163)</f>
+        <f t="shared" ref="L163:L194" si="4">ABS(K163-I163)</f>
         <v>0</v>
       </c>
     </row>
@@ -37454,7 +37460,7 @@
         <v>1</v>
       </c>
       <c r="L165" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -37504,7 +37510,7 @@
         <v>1</v>
       </c>
       <c r="L167" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -37555,7 +37561,7 @@
         <v>1</v>
       </c>
       <c r="L169" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -37612,13 +37618,13 @@
         <v>34</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>712</v>
+        <v>727</v>
       </c>
       <c r="H172" s="5">
-        <v>43</v>
+        <v>2124</v>
       </c>
       <c r="I172" s="7">
-        <v>3.5866210693135375E-3</v>
+        <v>0.17716239886562682</v>
       </c>
       <c r="J172" s="5">
         <v>1</v>
@@ -37628,21 +37634,21 @@
       </c>
       <c r="L172" s="8">
         <f>ABS(K172-I172)</f>
-        <v>0.12141337893068646</v>
+        <v>5.2162398865626819E-2</v>
       </c>
     </row>
     <row r="173" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>34</v>
       </c>
-      <c r="G173" s="22" t="s">
-        <v>492</v>
-      </c>
-      <c r="H173" s="23">
-        <v>216</v>
+      <c r="G173" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="H173" s="5">
+        <v>1004</v>
       </c>
       <c r="I173" s="7">
-        <v>1.8016515138877306E-2</v>
+        <v>8.3743431478855615E-2</v>
       </c>
       <c r="J173" s="5">
         <v>1</v>
@@ -37652,7 +37658,7 @@
       </c>
       <c r="L173" s="8">
         <f>ABS(K173-I173)</f>
-        <v>0.10698348486112269</v>
+        <v>4.1256568521144385E-2</v>
       </c>
     </row>
     <row r="174" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37660,13 +37666,13 @@
         <v>34</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>713</v>
+        <v>947</v>
       </c>
       <c r="H174" s="5">
-        <v>265</v>
+        <v>977</v>
       </c>
       <c r="I174" s="7">
-        <v>2.2103594962048546E-2</v>
+        <v>8.1491367086495958E-2</v>
       </c>
       <c r="J174" s="5">
         <v>1</v>
@@ -37676,7 +37682,7 @@
       </c>
       <c r="L174" s="8">
         <f>ABS(K174-I174)</f>
-        <v>0.10289640503795146</v>
+        <v>4.3508632913504042E-2</v>
       </c>
     </row>
     <row r="175" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37708,13 +37714,13 @@
         <v>34</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>727</v>
+        <v>713</v>
       </c>
       <c r="H176" s="5">
-        <v>2124</v>
+        <v>265</v>
       </c>
       <c r="I176" s="7">
-        <v>0.17716239886562682</v>
+        <v>2.2103594962048546E-2</v>
       </c>
       <c r="J176" s="5">
         <v>1</v>
@@ -37724,21 +37730,21 @@
       </c>
       <c r="L176" s="8">
         <f>ABS(K176-I176)</f>
-        <v>5.2162398865626819E-2</v>
+        <v>0.10289640503795146</v>
       </c>
     </row>
     <row r="177" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>34</v>
       </c>
-      <c r="G177" s="3" t="s">
-        <v>947</v>
-      </c>
-      <c r="H177" s="5">
-        <v>977</v>
+      <c r="G177" s="22" t="s">
+        <v>492</v>
+      </c>
+      <c r="H177" s="23">
+        <v>216</v>
       </c>
       <c r="I177" s="7">
-        <v>8.1491367086495958E-2</v>
+        <v>1.8016515138877306E-2</v>
       </c>
       <c r="J177" s="5">
         <v>1</v>
@@ -37748,7 +37754,7 @@
       </c>
       <c r="L177" s="8">
         <f>ABS(K177-I177)</f>
-        <v>4.3508632913504042E-2</v>
+        <v>0.10698348486112269</v>
       </c>
     </row>
     <row r="178" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37756,13 +37762,13 @@
         <v>34</v>
       </c>
       <c r="G178" s="3" t="s">
-        <v>977</v>
+        <v>712</v>
       </c>
       <c r="H178" s="5">
-        <v>1004</v>
+        <v>43</v>
       </c>
       <c r="I178" s="7">
-        <v>8.3743431478855615E-2</v>
+        <v>3.5866210693135375E-3</v>
       </c>
       <c r="J178" s="5">
         <v>1</v>
@@ -37772,7 +37778,7 @@
       </c>
       <c r="L178" s="8">
         <f>ABS(K178-I178)</f>
-        <v>4.1256568521144385E-2</v>
+        <v>0.12141337893068646</v>
       </c>
     </row>
     <row r="179" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -37861,13 +37867,13 @@
       <c r="C182" s="17"/>
       <c r="D182" s="16"/>
       <c r="G182" s="3" t="s">
-        <v>639</v>
+        <v>790</v>
       </c>
       <c r="H182" s="5">
-        <v>34</v>
+        <v>2551</v>
       </c>
       <c r="I182" s="7">
-        <v>2.8682301332883416E-3</v>
+        <v>0.2152016197064282</v>
       </c>
       <c r="J182" s="5">
         <v>1</v>
@@ -37877,7 +37883,7 @@
       </c>
       <c r="L182" s="8">
         <f>ABS(K182-I182)</f>
-        <v>0.10824288097782277</v>
+        <v>0.1040905085953171</v>
       </c>
     </row>
     <row r="183" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37888,13 +37894,13 @@
       <c r="C183" s="17"/>
       <c r="D183" s="16"/>
       <c r="G183" s="3" t="s">
-        <v>790</v>
+        <v>696</v>
       </c>
       <c r="H183" s="5">
-        <v>2551</v>
+        <v>868</v>
       </c>
       <c r="I183" s="7">
-        <v>0.2152016197064282</v>
+        <v>7.3224228108655309E-2</v>
       </c>
       <c r="J183" s="5">
         <v>1</v>
@@ -37904,7 +37910,7 @@
       </c>
       <c r="L183" s="8">
         <f>ABS(K183-I183)</f>
-        <v>0.1040905085953171</v>
+        <v>3.7886883002455796E-2</v>
       </c>
     </row>
     <row r="184" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37915,13 +37921,13 @@
       <c r="C184" s="17"/>
       <c r="D184" s="16"/>
       <c r="G184" s="3" t="s">
-        <v>655</v>
+        <v>857</v>
       </c>
       <c r="H184" s="5">
-        <v>286</v>
+        <v>804</v>
       </c>
       <c r="I184" s="7">
-        <v>2.4126877003543108E-2</v>
+        <v>6.782520668128901E-2</v>
       </c>
       <c r="J184" s="5">
         <v>1</v>
@@ -37931,7 +37937,7 @@
       </c>
       <c r="L184" s="8">
         <f>ABS(K184-I184)</f>
-        <v>8.6984234107568004E-2</v>
+        <v>4.3285904429822095E-2</v>
       </c>
     </row>
     <row r="185" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37942,13 +37948,13 @@
       <c r="C185" s="17"/>
       <c r="D185" s="16"/>
       <c r="G185" s="3" t="s">
-        <v>884</v>
+        <v>750</v>
       </c>
       <c r="H185" s="5">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="I185" s="7">
-        <v>2.699510713683145E-2</v>
+        <v>2.800742365446263E-2</v>
       </c>
       <c r="J185" s="5">
         <v>1</v>
@@ -37958,7 +37964,7 @@
       </c>
       <c r="L185" s="8">
         <f>ABS(K185-I185)</f>
-        <v>8.4116003974279652E-2</v>
+        <v>8.3103687456648478E-2</v>
       </c>
     </row>
     <row r="186" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37969,13 +37975,13 @@
       <c r="C186" s="17"/>
       <c r="D186" s="16"/>
       <c r="G186" s="3" t="s">
-        <v>750</v>
+        <v>884</v>
       </c>
       <c r="H186" s="5">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="I186" s="7">
-        <v>2.800742365446263E-2</v>
+        <v>2.699510713683145E-2</v>
       </c>
       <c r="J186" s="5">
         <v>1</v>
@@ -37985,7 +37991,7 @@
       </c>
       <c r="L186" s="8">
         <f>ABS(K186-I186)</f>
-        <v>8.3103687456648478E-2</v>
+        <v>8.4116003974279652E-2</v>
       </c>
     </row>
     <row r="187" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -37996,13 +38002,13 @@
       <c r="C187" s="17"/>
       <c r="D187" s="16"/>
       <c r="G187" s="3" t="s">
-        <v>857</v>
+        <v>655</v>
       </c>
       <c r="H187" s="5">
-        <v>804</v>
+        <v>286</v>
       </c>
       <c r="I187" s="7">
-        <v>6.782520668128901E-2</v>
+        <v>2.4126877003543108E-2</v>
       </c>
       <c r="J187" s="5">
         <v>1</v>
@@ -38012,7 +38018,7 @@
       </c>
       <c r="L187" s="8">
         <f>ABS(K187-I187)</f>
-        <v>4.3285904429822095E-2</v>
+        <v>8.6984234107568004E-2</v>
       </c>
     </row>
     <row r="188" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -38023,13 +38029,13 @@
       <c r="C188" s="17"/>
       <c r="D188" s="16"/>
       <c r="G188" s="3" t="s">
-        <v>696</v>
+        <v>639</v>
       </c>
       <c r="H188" s="5">
-        <v>868</v>
+        <v>34</v>
       </c>
       <c r="I188" s="7">
-        <v>7.3224228108655309E-2</v>
+        <v>2.8682301332883416E-3</v>
       </c>
       <c r="J188" s="5">
         <v>1</v>
@@ -38039,7 +38045,7 @@
       </c>
       <c r="L188" s="8">
         <f>ABS(K188-I188)</f>
-        <v>3.7886883002455796E-2</v>
+        <v>0.10824288097782277</v>
       </c>
     </row>
     <row r="189" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -38066,7 +38072,7 @@
       <c r="G189"/>
       <c r="H189" s="6"/>
     </row>
-    <row r="190" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>42</v>
       </c>
@@ -38089,11 +38095,11 @@
         <v>1</v>
       </c>
       <c r="L190" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>2399</v>
       </c>
@@ -38117,7 +38123,7 @@
       <c r="G191"/>
       <c r="H191" s="6"/>
     </row>
-    <row r="192" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>45</v>
       </c>
@@ -38140,11 +38146,11 @@
         <v>1</v>
       </c>
       <c r="L192" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>2400</v>
       </c>
@@ -38168,7 +38174,7 @@
       <c r="G193"/>
       <c r="H193" s="6"/>
     </row>
-    <row r="194" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>46</v>
       </c>
@@ -38191,11 +38197,11 @@
         <v>1</v>
       </c>
       <c r="L194" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>2401</v>
       </c>
@@ -38241,7 +38247,7 @@
         <v>1</v>
       </c>
       <c r="L196" s="8">
-        <f t="shared" ref="L196:L257" si="3">ABS(K196-I196)</f>
+        <f t="shared" ref="L196:L199" si="5">ABS(K196-I196)</f>
         <v>0</v>
       </c>
     </row>
@@ -38319,7 +38325,7 @@
         <v>0.5</v>
       </c>
       <c r="L199" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.2791815435319967</v>
       </c>
     </row>
@@ -38367,7 +38373,7 @@
         <v>0.6</v>
       </c>
       <c r="L201" s="8">
-        <f>ABS(K201-I201)</f>
+        <f t="shared" ref="L201:L219" si="6">ABS(K201-I201)</f>
         <v>0.56144436007761744</v>
       </c>
     </row>
@@ -38391,7 +38397,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L202" s="8">
-        <f>ABS(K202-I202)</f>
+        <f t="shared" si="6"/>
         <v>0.48892263561967436</v>
       </c>
     </row>
@@ -38415,7 +38421,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L203" s="8">
-        <f>ABS(K203-I203)</f>
+        <f t="shared" si="6"/>
         <v>0.18376782249219606</v>
       </c>
     </row>
@@ -38439,7 +38445,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L204" s="8">
-        <f>ABS(K204-I204)</f>
+        <f t="shared" si="6"/>
         <v>9.5671981776765377E-2</v>
       </c>
     </row>
@@ -38463,7 +38469,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L205" s="8">
-        <f>ABS(K205-I205)</f>
+        <f t="shared" si="6"/>
         <v>5.7909390027841054E-2</v>
       </c>
     </row>
@@ -38487,7 +38493,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L206" s="8">
-        <f>ABS(K206-I206)</f>
+        <f t="shared" si="6"/>
         <v>2.1935375010545856E-2</v>
       </c>
     </row>
@@ -38511,7 +38517,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L207" s="8">
-        <f>ABS(K207-I207)</f>
+        <f t="shared" si="6"/>
         <v>2.1884754914367671E-2</v>
       </c>
     </row>
@@ -38535,7 +38541,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L208" s="8">
-        <f>ABS(K208-I208)</f>
+        <f t="shared" si="6"/>
         <v>2.1209820298658567E-2</v>
       </c>
     </row>
@@ -38559,7 +38565,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L209" s="8">
-        <f>ABS(K209-I209)</f>
+        <f t="shared" si="6"/>
         <v>2.1024213279338566E-2</v>
       </c>
     </row>
@@ -38583,7 +38589,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L210" s="8">
-        <f>ABS(K210-I210)</f>
+        <f t="shared" si="6"/>
         <v>2.0956719817767654E-2</v>
       </c>
     </row>
@@ -38607,7 +38613,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L211" s="8">
-        <f>ABS(K211-I211)</f>
+        <f t="shared" si="6"/>
         <v>2.0804859529233107E-2</v>
       </c>
     </row>
@@ -38631,7 +38637,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L212" s="8">
-        <f>ABS(K212-I212)</f>
+        <f t="shared" si="6"/>
         <v>2.0602379144520375E-2</v>
       </c>
     </row>
@@ -38655,7 +38661,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L213" s="8">
-        <f>ABS(K213-I213)</f>
+        <f t="shared" si="6"/>
         <v>2.0551759048342194E-2</v>
       </c>
     </row>
@@ -38679,7 +38685,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L214" s="8">
-        <f>ABS(K214-I214)</f>
+        <f t="shared" si="6"/>
         <v>2.0501138952164009E-2</v>
       </c>
     </row>
@@ -38703,7 +38709,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L215" s="8">
-        <f>ABS(K215-I215)</f>
+        <f t="shared" si="6"/>
         <v>1.9522483759385811E-2</v>
       </c>
     </row>
@@ -38727,7 +38733,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L216" s="8">
-        <f>ABS(K216-I216)</f>
+        <f t="shared" si="6"/>
         <v>1.8712562220534888E-2</v>
       </c>
     </row>
@@ -38751,7 +38757,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L217" s="8">
-        <f>ABS(K217-I217)</f>
+        <f t="shared" si="6"/>
         <v>1.8577575297393067E-2</v>
       </c>
     </row>
@@ -38775,7 +38781,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L218" s="8">
-        <f>ABS(K218-I218)</f>
+        <f t="shared" si="6"/>
         <v>1.6620264911836668E-2</v>
       </c>
     </row>
@@ -38799,7 +38805,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L219" s="8">
-        <f>ABS(K219-I219)</f>
+        <f t="shared" si="6"/>
         <v>1.9235636547709455E-3</v>
       </c>
     </row>
@@ -38847,7 +38853,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L221" s="8">
-        <f>ABS(K221-I221)</f>
+        <f t="shared" ref="L221:L237" si="7">ABS(K221-I221)</f>
         <v>0.93639099516990132</v>
       </c>
     </row>
@@ -38871,7 +38877,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L222" s="8">
-        <f>ABS(K222-I222)</f>
+        <f t="shared" si="7"/>
         <v>5.880456451578716E-2</v>
       </c>
     </row>
@@ -38895,7 +38901,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L223" s="8">
-        <f>ABS(K223-I223)</f>
+        <f t="shared" si="7"/>
         <v>5.8798242883794642E-2</v>
       </c>
     </row>
@@ -38919,7 +38925,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L224" s="8">
-        <f>ABS(K224-I224)</f>
+        <f t="shared" si="7"/>
         <v>5.8798242883794642E-2</v>
       </c>
     </row>
@@ -38943,7 +38949,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L225" s="8">
-        <f>ABS(K225-I225)</f>
+        <f t="shared" si="7"/>
         <v>5.8798242883794642E-2</v>
       </c>
     </row>
@@ -38967,7 +38973,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L226" s="8">
-        <f>ABS(K226-I226)</f>
+        <f t="shared" si="7"/>
         <v>5.8791921251802132E-2</v>
       </c>
     </row>
@@ -38991,7 +38997,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L227" s="8">
-        <f>ABS(K227-I227)</f>
+        <f t="shared" si="7"/>
         <v>5.8772956355824586E-2</v>
       </c>
     </row>
@@ -39015,7 +39021,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L228" s="8">
-        <f>ABS(K228-I228)</f>
+        <f t="shared" si="7"/>
         <v>5.8772956355824586E-2</v>
       </c>
     </row>
@@ -39039,7 +39045,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L229" s="8">
-        <f>ABS(K229-I229)</f>
+        <f t="shared" si="7"/>
         <v>5.8753991459847041E-2</v>
       </c>
     </row>
@@ -39063,7 +39069,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L230" s="8">
-        <f>ABS(K230-I230)</f>
+        <f t="shared" si="7"/>
         <v>5.8728704931876978E-2</v>
       </c>
     </row>
@@ -39087,7 +39093,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L231" s="8">
-        <f>ABS(K231-I231)</f>
+        <f t="shared" si="7"/>
         <v>5.8583307396049125E-2</v>
       </c>
     </row>
@@ -39111,7 +39117,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L232" s="8">
-        <f>ABS(K232-I232)</f>
+        <f t="shared" si="7"/>
         <v>5.8539055972101524E-2</v>
       </c>
     </row>
@@ -39135,7 +39141,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L233" s="8">
-        <f>ABS(K233-I233)</f>
+        <f t="shared" si="7"/>
         <v>5.8488482916161398E-2</v>
       </c>
     </row>
@@ -39159,7 +39165,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L234" s="8">
-        <f>ABS(K234-I234)</f>
+        <f t="shared" si="7"/>
         <v>5.8450553124206307E-2</v>
       </c>
     </row>
@@ -39183,7 +39189,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L235" s="8">
-        <f>ABS(K235-I235)</f>
+        <f t="shared" si="7"/>
         <v>5.8343085380333552E-2</v>
       </c>
     </row>
@@ -39207,7 +39213,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L236" s="8">
-        <f>ABS(K236-I236)</f>
+        <f t="shared" si="7"/>
         <v>5.7514951589314064E-2</v>
       </c>
     </row>
@@ -39231,7 +39237,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L237" s="8">
-        <f>ABS(K237-I237)</f>
+        <f t="shared" si="7"/>
         <v>5.7451735269388911E-2</v>
       </c>
     </row>
@@ -39282,7 +39288,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L239" s="8">
-        <f>ABS(K239-I239)</f>
+        <f t="shared" ref="L239:L251" si="8">ABS(K239-I239)</f>
         <v>0.20167883325778063</v>
       </c>
     </row>
@@ -39309,7 +39315,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L240" s="8">
-        <f>ABS(K240-I240)</f>
+        <f t="shared" si="8"/>
         <v>0.15941100151626467</v>
       </c>
     </row>
@@ -39336,7 +39342,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L241" s="8">
-        <f>ABS(K241-I241)</f>
+        <f t="shared" si="8"/>
         <v>0.11822696033222349</v>
       </c>
     </row>
@@ -39363,7 +39369,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L242" s="8">
-        <f>ABS(K242-I242)</f>
+        <f t="shared" si="8"/>
         <v>7.6042497095128683E-2</v>
       </c>
     </row>
@@ -39390,7 +39396,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L243" s="8">
-        <f>ABS(K243-I243)</f>
+        <f t="shared" si="8"/>
         <v>7.5263522631943691E-2</v>
       </c>
     </row>
@@ -39417,7 +39423,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L244" s="8">
-        <f>ABS(K244-I244)</f>
+        <f t="shared" si="8"/>
         <v>7.5128048812259346E-2</v>
       </c>
     </row>
@@ -39444,7 +39450,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L245" s="8">
-        <f>ABS(K245-I245)</f>
+        <f t="shared" si="8"/>
         <v>7.1910545594756126E-2</v>
       </c>
     </row>
@@ -39471,7 +39477,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L246" s="8">
-        <f>ABS(K246-I246)</f>
+        <f t="shared" si="8"/>
         <v>6.8218884008357697E-2</v>
       </c>
     </row>
@@ -39498,7 +39504,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L247" s="8">
-        <f>ABS(K247-I247)</f>
+        <f t="shared" si="8"/>
         <v>6.3985327143221887E-2</v>
       </c>
     </row>
@@ -39525,7 +39531,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L248" s="8">
-        <f>ABS(K248-I248)</f>
+        <f t="shared" si="8"/>
         <v>4.5899572215361693E-2</v>
       </c>
     </row>
@@ -39552,7 +39558,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L249" s="8">
-        <f>ABS(K249-I249)</f>
+        <f t="shared" si="8"/>
         <v>1.612920033972666E-2</v>
       </c>
     </row>
@@ -39579,7 +39585,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L250" s="8">
-        <f>ABS(K250-I250)</f>
+        <f t="shared" si="8"/>
         <v>7.3416389205862853E-3</v>
       </c>
     </row>
@@ -39606,7 +39612,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L251" s="8">
-        <f>ABS(K251-I251)</f>
+        <f t="shared" si="8"/>
         <v>5.9191638139006464E-3</v>
       </c>
     </row>
@@ -39801,7 +39807,7 @@
         <v>1</v>
       </c>
       <c r="L259" s="8">
-        <f t="shared" ref="L259:L302" si="4">ABS(K259-I259)</f>
+        <f t="shared" ref="L259:L302" si="9">ABS(K259-I259)</f>
         <v>0</v>
       </c>
     </row>
@@ -39851,7 +39857,7 @@
         <v>1</v>
       </c>
       <c r="L261" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -39899,7 +39905,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L263" s="8">
-        <f>ABS(K263-I263)</f>
+        <f t="shared" ref="L263:L283" si="10">ABS(K263-I263)</f>
         <v>0.68903650353175805</v>
       </c>
     </row>
@@ -39923,7 +39929,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L264" s="8">
-        <f>ABS(K264-I264)</f>
+        <f t="shared" si="10"/>
         <v>8.7959153532924023E-2</v>
       </c>
     </row>
@@ -39947,7 +39953,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L265" s="8">
-        <f>ABS(K265-I265)</f>
+        <f t="shared" si="10"/>
         <v>4.7269258658387214E-2</v>
       </c>
     </row>
@@ -39971,7 +39977,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L266" s="8">
-        <f>ABS(K266-I266)</f>
+        <f t="shared" si="10"/>
         <v>4.7245939394343191E-2</v>
       </c>
     </row>
@@ -39995,7 +40001,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L267" s="8">
-        <f>ABS(K267-I267)</f>
+        <f t="shared" si="10"/>
         <v>4.7245939394343191E-2</v>
       </c>
     </row>
@@ -40019,7 +40025,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L268" s="8">
-        <f>ABS(K268-I268)</f>
+        <f t="shared" si="10"/>
         <v>4.7082704546034998E-2</v>
       </c>
     </row>
@@ -40043,7 +40049,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L269" s="8">
-        <f>ABS(K269-I269)</f>
+        <f t="shared" si="10"/>
         <v>4.6966108225814866E-2</v>
       </c>
     </row>
@@ -40067,7 +40073,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L270" s="8">
-        <f>ABS(K270-I270)</f>
+        <f t="shared" si="10"/>
         <v>4.6289849568538093E-2</v>
       </c>
     </row>
@@ -40091,7 +40097,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L271" s="8">
-        <f>ABS(K271-I271)</f>
+        <f t="shared" si="10"/>
         <v>4.6056656928097822E-2</v>
       </c>
     </row>
@@ -40115,7 +40121,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L272" s="8">
-        <f>ABS(K272-I272)</f>
+        <f t="shared" si="10"/>
         <v>4.594006060787769E-2</v>
       </c>
     </row>
@@ -40139,7 +40145,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L273" s="8">
-        <f>ABS(K273-I273)</f>
+        <f t="shared" si="10"/>
         <v>4.5473675326997157E-2</v>
       </c>
     </row>
@@ -40163,7 +40169,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L274" s="8">
-        <f>ABS(K274-I274)</f>
+        <f t="shared" si="10"/>
         <v>4.4610862557368167E-2</v>
       </c>
     </row>
@@ -40187,7 +40193,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L275" s="8">
-        <f>ABS(K275-I275)</f>
+        <f t="shared" si="10"/>
         <v>4.4587543293324136E-2</v>
       </c>
     </row>
@@ -40211,7 +40217,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L276" s="8">
-        <f>ABS(K276-I276)</f>
+        <f t="shared" si="10"/>
         <v>4.4377669916927896E-2</v>
       </c>
     </row>
@@ -40235,7 +40241,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L277" s="8">
-        <f>ABS(K277-I277)</f>
+        <f t="shared" si="10"/>
         <v>4.4027880956267494E-2</v>
       </c>
     </row>
@@ -40259,7 +40265,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L278" s="8">
-        <f>ABS(K278-I278)</f>
+        <f t="shared" si="10"/>
         <v>4.311842965855045E-2</v>
       </c>
     </row>
@@ -40283,7 +40289,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L279" s="8">
-        <f>ABS(K279-I279)</f>
+        <f t="shared" si="10"/>
         <v>3.901423918680174E-2</v>
       </c>
     </row>
@@ -40307,7 +40313,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L280" s="8">
-        <f>ABS(K280-I280)</f>
+        <f t="shared" si="10"/>
         <v>3.8221384209304828E-2</v>
       </c>
     </row>
@@ -40331,7 +40337,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L281" s="8">
-        <f>ABS(K281-I281)</f>
+        <f t="shared" si="10"/>
         <v>3.5446391788065641E-2</v>
       </c>
     </row>
@@ -40355,7 +40361,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L282" s="8">
-        <f>ABS(K282-I282)</f>
+        <f t="shared" si="10"/>
         <v>1.3946030339472962E-2</v>
       </c>
     </row>
@@ -40379,7 +40385,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L283" s="8">
-        <f>ABS(K283-I283)</f>
+        <f t="shared" si="10"/>
         <v>1.0075032508164515E-2</v>
       </c>
     </row>
@@ -40427,7 +40433,7 @@
         <v>1</v>
       </c>
       <c r="L285" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -40475,7 +40481,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L287" s="8">
-        <f>ABS(K287-I287)</f>
+        <f t="shared" ref="L287:L298" si="11">ABS(K287-I287)</f>
         <v>0.15660935942220902</v>
       </c>
     </row>
@@ -40499,7 +40505,7 @@
         <v>0.42857142857142855</v>
       </c>
       <c r="L288" s="8">
-        <f>ABS(K288-I288)</f>
+        <f t="shared" si="11"/>
         <v>0.13954656499006823</v>
       </c>
     </row>
@@ -40523,7 +40529,7 @@
         <v>9.5238095238095233E-2</v>
       </c>
       <c r="L289" s="8">
-        <f>ABS(K289-I289)</f>
+        <f t="shared" si="11"/>
         <v>7.8441669140086906E-2</v>
       </c>
     </row>
@@ -40547,7 +40553,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L290" s="8">
-        <f>ABS(K290-I290)</f>
+        <f t="shared" si="11"/>
         <v>4.0632586740945373E-2</v>
       </c>
     </row>
@@ -40571,7 +40577,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L291" s="8">
-        <f>ABS(K291-I291)</f>
+        <f t="shared" si="11"/>
         <v>3.9483397642259721E-2</v>
       </c>
     </row>
@@ -40595,7 +40601,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L292" s="8">
-        <f>ABS(K292-I292)</f>
+        <f t="shared" si="11"/>
         <v>3.6500072299976406E-2</v>
       </c>
     </row>
@@ -40619,7 +40625,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L293" s="8">
-        <f>ABS(K293-I293)</f>
+        <f t="shared" si="11"/>
         <v>3.5084514867158301E-2</v>
       </c>
     </row>
@@ -40643,7 +40649,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L294" s="8">
-        <f>ABS(K294-I294)</f>
+        <f t="shared" si="11"/>
         <v>2.5015791836952135E-2</v>
       </c>
     </row>
@@ -40667,7 +40673,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L295" s="8">
-        <f>ABS(K295-I295)</f>
+        <f t="shared" si="11"/>
         <v>2.4460223597190203E-2</v>
       </c>
     </row>
@@ -40691,7 +40697,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L296" s="8">
-        <f>ABS(K296-I296)</f>
+        <f t="shared" si="11"/>
         <v>2.2755466258742585E-2</v>
       </c>
     </row>
@@ -40715,7 +40721,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L297" s="8">
-        <f>ABS(K297-I297)</f>
+        <f t="shared" si="11"/>
         <v>1.224533284625981E-2</v>
       </c>
     </row>
@@ -40739,7 +40745,7 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L298" s="8">
-        <f>ABS(K298-I298)</f>
+        <f t="shared" si="11"/>
         <v>1.1704985654162572E-2</v>
       </c>
     </row>
@@ -40789,7 +40795,7 @@
         <v>1</v>
       </c>
       <c r="L300" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -40840,7 +40846,7 @@
         <v>1</v>
       </c>
       <c r="L302" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -41253,9 +41259,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="G287:L298">
-    <sortCondition descending="1" ref="L287:L298"/>
+  <sortState ref="G180:L188">
+    <sortCondition descending="1" ref="H180:H188"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Beginning a summary document for spread vs. usage analysis
</commit_message>
<xml_diff>
--- a/untl-bs/data/SpreadVsUsage-2022-09-15.xlsx
+++ b/untl-bs/data/SpreadVsUsage-2022-09-15.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hjones\Documents\GitHub\portal-leading\untl-bs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C27BBE6-654C-4403-AD4C-CA356B0C7791}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457B6B4F-9B7D-471F-98B9-AED403F6E2FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{EC6FB916-47AD-4345-B293-575366B1C3FF}"/>
   </bookViews>
@@ -7363,7 +7363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7427,6 +7427,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -33329,8 +33332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFD2735-90EA-4E93-A47B-4BEF3700C1A2}">
   <dimension ref="A1:L664"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="G189" sqref="G189"/>
+    <sheetView tabSelected="1" topLeftCell="F67" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77:L90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -33387,7 +33390,7 @@
         <v>2417</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -33397,7 +33400,7 @@
       <c r="H2" s="23">
         <v>5996</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="25">
         <v>0.34509352517985614</v>
       </c>
       <c r="J2" s="5">
@@ -33411,7 +33414,7 @@
         <v>0.2541844342707652</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -33435,7 +33438,7 @@
         <v>0.16572400261608897</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -33459,7 +33462,7 @@
         <v>0.13157357750163506</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -33483,7 +33486,7 @@
         <v>9.7491170699803786E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -33507,7 +33510,7 @@
         <v>8.3369522563767173E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -33531,7 +33534,7 @@
         <v>8.2333551340745589E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -33555,7 +33558,7 @@
         <v>7.640549378678875E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -33579,7 +33582,7 @@
         <v>7.5829954218443435E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -33603,7 +33606,7 @@
         <v>6.7887508175277958E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2378</v>
       </c>
@@ -33627,7 +33630,7 @@
       <c r="G11"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -33637,7 +33640,7 @@
       <c r="H12" s="23">
         <v>2769</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="25">
         <v>0.31820271202022521</v>
       </c>
       <c r="J12" s="5">
@@ -33647,11 +33650,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L12" s="8">
-        <f>ABS(K12-I12)</f>
+        <f t="shared" ref="L12:L28" si="1">ABS(K12-I12)</f>
         <v>0.25937918260846049</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -33671,11 +33674,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L13" s="8">
-        <f>ABS(K13-I13)</f>
+        <f t="shared" si="1"/>
         <v>0.16756120972866279</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -33695,11 +33698,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L14" s="8">
-        <f>ABS(K14-I14)</f>
+        <f t="shared" si="1"/>
         <v>3.8050752362540047E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -33719,11 +33722,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L15" s="8">
-        <f>ABS(K15-I15)</f>
+        <f t="shared" si="1"/>
         <v>2.0813335676720696E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -33743,11 +33746,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L16" s="8">
-        <f>ABS(K16-I16)</f>
+        <f t="shared" si="1"/>
         <v>9.5245176903213588E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -33767,11 +33770,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L17" s="8">
-        <f>ABS(K17-I17)</f>
+        <f t="shared" si="1"/>
         <v>1.4810658807305963E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -33791,11 +33794,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L18" s="8">
-        <f>ABS(K18-I18)</f>
+        <f t="shared" si="1"/>
         <v>2.0096799924290559E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -33815,11 +33818,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L19" s="8">
-        <f>ABS(K19-I19)</f>
+        <f t="shared" si="1"/>
         <v>2.2165289926588887E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -33839,11 +33842,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L20" s="8">
-        <f>ABS(K20-I20)</f>
+        <f t="shared" si="1"/>
         <v>2.6876850487379506E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -33863,11 +33866,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L21" s="8">
-        <f>ABS(K21-I21)</f>
+        <f t="shared" si="1"/>
         <v>3.9747454946124625E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -33887,11 +33890,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L22" s="8">
-        <f>ABS(K22-I22)</f>
+        <f t="shared" si="1"/>
         <v>4.4229183284437652E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -33911,11 +33914,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L23" s="8">
-        <f>ABS(K23-I23)</f>
+        <f t="shared" si="1"/>
         <v>4.8825827733989483E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -33935,11 +33938,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L24" s="8">
-        <f>ABS(K24-I24)</f>
+        <f t="shared" si="1"/>
         <v>4.9055659956467074E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -33959,11 +33962,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L25" s="8">
-        <f>ABS(K25-I25)</f>
+        <f t="shared" si="1"/>
         <v>4.9515324401422256E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -33983,11 +33986,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L26" s="8">
-        <f>ABS(K26-I26)</f>
+        <f t="shared" si="1"/>
         <v>5.2503143293630941E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -34007,11 +34010,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L27" s="8">
-        <f>ABS(K27-I27)</f>
+        <f t="shared" si="1"/>
         <v>5.2847891627347328E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -34031,11 +34034,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L28" s="8">
-        <f>ABS(K28-I28)</f>
+        <f t="shared" si="1"/>
         <v>5.5605878297078429E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>2379</v>
       </c>
@@ -34059,7 +34062,7 @@
       <c r="G29"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -34069,7 +34072,7 @@
       <c r="H30" s="23">
         <v>115444</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="25">
         <v>1</v>
       </c>
       <c r="J30" s="5">
@@ -34079,11 +34082,11 @@
         <v>1</v>
       </c>
       <c r="L30" s="8">
-        <f t="shared" ref="L30:L60" si="1">ABS(K30-I30)</f>
+        <f t="shared" ref="L30:L60" si="2">ABS(K30-I30)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2380</v>
       </c>
@@ -34107,7 +34110,7 @@
       <c r="G31"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -34131,7 +34134,7 @@
         <v>0.53534094842506064</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -34155,7 +34158,7 @@
         <v>0.31242644513672552</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -34165,7 +34168,7 @@
       <c r="H34" s="23">
         <v>793</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="25">
         <v>5.4897888542748359E-2</v>
       </c>
       <c r="J34" s="5">
@@ -34179,7 +34182,7 @@
         <v>0.14510211145725166</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -34203,7 +34206,7 @@
         <v>7.7812391831083433E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>2381</v>
       </c>
@@ -34227,7 +34230,7 @@
       <c r="G36"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -34254,7 +34257,7 @@
         <v>0.33844613114062827</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -34267,7 +34270,7 @@
       <c r="H38" s="23">
         <v>1179</v>
       </c>
-      <c r="I38" s="7">
+      <c r="I38" s="25">
         <v>0.24857685009487665</v>
       </c>
       <c r="J38" s="5">
@@ -34281,7 +34284,7 @@
         <v>1.4231499051233498E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -34308,7 +34311,7 @@
         <v>0.13277461522243306</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -34335,7 +34338,7 @@
         <v>0.20424836601307189</v>
       </c>
     </row>
-    <row r="41" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>2382</v>
       </c>
@@ -34359,7 +34362,7 @@
       <c r="G41"/>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -34382,11 +34385,11 @@
         <v>0.45454545454545453</v>
       </c>
       <c r="L42" s="8">
-        <f>ABS(K42-I42)</f>
+        <f t="shared" ref="L42:L48" si="3">ABS(K42-I42)</f>
         <v>1.6911731233213489E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -34409,11 +34412,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L43" s="8">
-        <f>ABS(K43-I43)</f>
+        <f t="shared" si="3"/>
         <v>0.10112896617653752</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -34426,7 +34429,7 @@
       <c r="H44" s="23">
         <v>595</v>
       </c>
-      <c r="I44" s="7">
+      <c r="I44" s="25">
         <v>0.14897346019028543</v>
       </c>
       <c r="J44" s="5">
@@ -34436,11 +34439,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L44" s="8">
-        <f>ABS(K44-I44)</f>
+        <f t="shared" si="3"/>
         <v>5.8064369281194517E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>35</v>
       </c>
@@ -34463,11 +34466,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L45" s="8">
-        <f>ABS(K45-I45)</f>
+        <f t="shared" si="3"/>
         <v>1.5045295215550605E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -34490,11 +34493,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L46" s="8">
-        <f>ABS(K46-I46)</f>
+        <f t="shared" si="3"/>
         <v>4.0833978240087408E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -34517,11 +34520,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L47" s="8">
-        <f>ABS(K47-I47)</f>
+        <f t="shared" si="3"/>
         <v>5.2601629717303228E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -34544,11 +34547,11 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="L48" s="8">
-        <f>ABS(K48-I48)</f>
+        <f t="shared" si="3"/>
         <v>6.7624163518004279E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>2383</v>
       </c>
@@ -34572,7 +34575,7 @@
       <c r="G49"/>
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -34582,7 +34585,7 @@
       <c r="H50" s="23">
         <v>67422</v>
       </c>
-      <c r="I50" s="7">
+      <c r="I50" s="25">
         <v>0.84170183016653766</v>
       </c>
       <c r="J50" s="5">
@@ -34592,11 +34595,11 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="L50" s="8">
-        <f>ABS(K50-I50)</f>
+        <f t="shared" ref="L50:L55" si="4">ABS(K50-I50)</f>
         <v>0.67503516349987103</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -34616,11 +34619,11 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="L51" s="8">
-        <f>ABS(K51-I51)</f>
+        <f t="shared" si="4"/>
         <v>0.10846587267900093</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -34640,11 +34643,11 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="L52" s="8">
-        <f>ABS(K52-I52)</f>
+        <f t="shared" si="4"/>
         <v>0.11721721471790134</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -34664,11 +34667,11 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="L53" s="8">
-        <f>ABS(K53-I53)</f>
+        <f t="shared" si="4"/>
         <v>0.14503175118390718</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -34688,11 +34691,11 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="L54" s="8">
-        <f>ABS(K54-I54)</f>
+        <f t="shared" si="4"/>
         <v>0.15127379258112572</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>26</v>
       </c>
@@ -34712,11 +34715,11 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="L55" s="8">
-        <f>ABS(K55-I55)</f>
+        <f t="shared" si="4"/>
         <v>0.1530465323379358</v>
       </c>
     </row>
-    <row r="56" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>2384</v>
       </c>
@@ -34740,7 +34743,7 @@
       <c r="G56"/>
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>37</v>
       </c>
@@ -34753,7 +34756,7 @@
       <c r="H57" s="23">
         <v>21109</v>
       </c>
-      <c r="I57" s="7">
+      <c r="I57" s="25">
         <v>0.75792610678252126</v>
       </c>
       <c r="J57" s="5">
@@ -34767,7 +34770,7 @@
         <v>0.25792610678252126</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>37</v>
       </c>
@@ -34790,11 +34793,11 @@
         <v>0.5</v>
       </c>
       <c r="L58" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25792610678252126</v>
       </c>
     </row>
-    <row r="59" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>2385</v>
       </c>
@@ -34818,7 +34821,7 @@
       <c r="G59"/>
       <c r="H59" s="6"/>
     </row>
-    <row r="60" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -34841,11 +34844,11 @@
         <v>1</v>
       </c>
       <c r="L60" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>2386</v>
       </c>
@@ -34869,7 +34872,7 @@
       <c r="G61"/>
       <c r="H61" s="6"/>
     </row>
-    <row r="62" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>36</v>
       </c>
@@ -34896,7 +34899,7 @@
         <v>0.526192279295147</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -34923,7 +34926,7 @@
         <v>2.931186554330234E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>36</v>
       </c>
@@ -34950,7 +34953,7 @@
         <v>0.24807782156725772</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>36</v>
       </c>
@@ -34963,7 +34966,7 @@
       <c r="H65" s="23">
         <v>1325</v>
       </c>
-      <c r="I65" s="7">
+      <c r="I65" s="25">
         <v>1.1974078154130335E-3</v>
       </c>
       <c r="J65" s="5">
@@ -34977,7 +34980,7 @@
         <v>0.24880259218458697</v>
       </c>
     </row>
-    <row r="66" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>2387</v>
       </c>
@@ -35001,7 +35004,7 @@
       <c r="G66"/>
       <c r="H66" s="6"/>
     </row>
-    <row r="67" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -35014,7 +35017,7 @@
       <c r="H67" s="23">
         <v>848333</v>
       </c>
-      <c r="I67" s="7">
+      <c r="I67" s="25">
         <v>1</v>
       </c>
       <c r="J67" s="5">
@@ -35024,11 +35027,11 @@
         <v>1</v>
       </c>
       <c r="L67" s="8">
-        <f t="shared" ref="L67" si="2">ABS(K67-I67)</f>
+        <f t="shared" ref="L67" si="5">ABS(K67-I67)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>2388</v>
       </c>
@@ -35052,7 +35055,7 @@
       <c r="G68"/>
       <c r="H68" s="6"/>
     </row>
-    <row r="69" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>32</v>
       </c>
@@ -35062,7 +35065,7 @@
       <c r="H69" s="23">
         <v>3444</v>
       </c>
-      <c r="I69" s="7">
+      <c r="I69" s="25">
         <v>0.30935057935866345</v>
       </c>
       <c r="J69" s="5">
@@ -35072,11 +35075,11 @@
         <v>6.25E-2</v>
       </c>
       <c r="L69" s="8">
-        <f t="shared" ref="L69:L75" si="3">ABS(K69-I69)</f>
+        <f t="shared" ref="L69:L75" si="6">ABS(K69-I69)</f>
         <v>0.24685057935866345</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>32</v>
       </c>
@@ -35096,11 +35099,11 @@
         <v>0.5</v>
       </c>
       <c r="L70" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.18552950687146319</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -35120,11 +35123,11 @@
         <v>0.1875</v>
       </c>
       <c r="L71" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.16190043115063324</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>32</v>
       </c>
@@ -35144,11 +35147,11 @@
         <v>6.25E-2</v>
       </c>
       <c r="L72" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.11463105182789904</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>32</v>
       </c>
@@ -35168,11 +35171,11 @@
         <v>6.25E-2</v>
       </c>
       <c r="L73" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.9565481002425221E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>32</v>
       </c>
@@ -35192,11 +35195,11 @@
         <v>6.25E-2</v>
       </c>
       <c r="L74" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.9000044911524298E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>32</v>
       </c>
@@ -35216,11 +35219,11 @@
         <v>6.25E-2</v>
       </c>
       <c r="L75" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.4862570735650772E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>2389</v>
       </c>
@@ -35244,7 +35247,7 @@
       <c r="G76"/>
       <c r="H76" s="6"/>
     </row>
-    <row r="77" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>24</v>
       </c>
@@ -35257,7 +35260,7 @@
       <c r="H77" s="23">
         <v>5327</v>
       </c>
-      <c r="I77" s="7">
+      <c r="I77" s="25">
         <v>0.45894718704230208</v>
       </c>
       <c r="J77" s="5">
@@ -35267,11 +35270,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L77" s="8">
-        <f>ABS(K77-I77)</f>
+        <f t="shared" ref="L77:L90" si="7">ABS(K77-I77)</f>
         <v>0.38751861561373069</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>24</v>
       </c>
@@ -35294,11 +35297,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L78" s="8">
-        <f>ABS(K78-I78)</f>
+        <f t="shared" si="7"/>
         <v>8.8819554702211728E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>24</v>
       </c>
@@ -35321,11 +35324,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L79" s="8">
-        <f>ABS(K79-I79)</f>
+        <f t="shared" si="7"/>
         <v>2.3427980652069566E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -35348,11 +35351,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L80" s="8">
-        <f>ABS(K80-I80)</f>
+        <f t="shared" si="7"/>
         <v>1.5944811628450808E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>24</v>
       </c>
@@ -35375,11 +35378,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L81" s="8">
-        <f>ABS(K81-I81)</f>
+        <f t="shared" si="7"/>
         <v>3.0160371204568666E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>24</v>
       </c>
@@ -35402,11 +35405,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L82" s="8">
-        <f>ABS(K82-I82)</f>
+        <f t="shared" si="7"/>
         <v>3.3520412558923796E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>24</v>
       </c>
@@ -35429,11 +35432,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L83" s="8">
-        <f>ABS(K83-I83)</f>
+        <f t="shared" si="7"/>
         <v>4.4806705313296155E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>24</v>
       </c>
@@ -35456,11 +35459,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L84" s="8">
-        <f>ABS(K84-I84)</f>
+        <f t="shared" si="7"/>
         <v>4.7132887789388178E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -35483,11 +35486,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L85" s="8">
-        <f>ABS(K85-I85)</f>
+        <f t="shared" si="7"/>
         <v>4.7649817228519728E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>24</v>
       </c>
@@ -35510,11 +35513,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L86" s="8">
-        <f>ABS(K86-I86)</f>
+        <f t="shared" si="7"/>
         <v>5.3508350872010724E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>24</v>
       </c>
@@ -35537,11 +35540,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L87" s="8">
-        <f>ABS(K87-I87)</f>
+        <f t="shared" si="7"/>
         <v>5.4800674469839626E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>24</v>
       </c>
@@ -35564,11 +35567,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L88" s="8">
-        <f>ABS(K88-I88)</f>
+        <f t="shared" si="7"/>
         <v>5.583453334810274E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>24</v>
       </c>
@@ -35591,11 +35594,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L89" s="8">
-        <f>ABS(K89-I89)</f>
+        <f t="shared" si="7"/>
         <v>5.6006843161146597E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>24</v>
       </c>
@@ -35618,11 +35621,11 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="L90" s="8">
-        <f>ABS(K90-I90)</f>
+        <f t="shared" si="7"/>
         <v>6.040074339376484E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>2390</v>
       </c>
@@ -35646,7 +35649,7 @@
       <c r="G91"/>
       <c r="H91" s="6"/>
     </row>
-    <row r="92" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>19</v>
       </c>
@@ -35669,11 +35672,11 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="L92" s="8">
-        <f>ABS(K92-I92)</f>
+        <f t="shared" ref="L92:L104" si="8">ABS(K92-I92)</f>
         <v>0.21939686271582823</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -35696,11 +35699,11 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="L93" s="8">
-        <f>ABS(K93-I93)</f>
+        <f t="shared" si="8"/>
         <v>6.6427825048514716E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>19</v>
       </c>
@@ -35723,11 +35726,11 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="L94" s="8">
-        <f>ABS(K94-I94)</f>
+        <f t="shared" si="8"/>
         <v>1.0150768771458429E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>19</v>
       </c>
@@ -35750,11 +35753,11 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="L95" s="8">
-        <f>ABS(K95-I95)</f>
+        <f t="shared" si="8"/>
         <v>4.7948698810767784E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>19</v>
       </c>
@@ -35767,7 +35770,7 @@
       <c r="H96" s="23">
         <v>4658</v>
       </c>
-      <c r="I96" s="7">
+      <c r="I96" s="25">
         <v>6.5186968204209578E-2</v>
       </c>
       <c r="J96" s="5">
@@ -35777,11 +35780,11 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="L96" s="8">
-        <f>ABS(K96-I96)</f>
+        <f t="shared" si="8"/>
         <v>9.6314126486540252E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>19</v>
       </c>
@@ -35804,11 +35807,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="L97" s="8">
-        <f>ABS(K97-I97)</f>
+        <f t="shared" si="8"/>
         <v>6.6258334577300099E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>19</v>
       </c>
@@ -35831,11 +35834,11 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="L98" s="8">
-        <f>ABS(K98-I98)</f>
+        <f t="shared" si="8"/>
         <v>2.0988829178484346E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>19</v>
       </c>
@@ -35858,11 +35861,11 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="L99" s="8">
-        <f>ABS(K99-I99)</f>
+        <f t="shared" si="8"/>
         <v>2.6376760212967105E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>19</v>
       </c>
@@ -35885,11 +35888,11 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="L100" s="8">
-        <f>ABS(K100-I100)</f>
+        <f t="shared" si="8"/>
         <v>3.0001368363437326E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>19</v>
       </c>
@@ -35912,11 +35915,11 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="L101" s="8">
-        <f>ABS(K101-I101)</f>
+        <f t="shared" si="8"/>
         <v>4.1602913370154745E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>19</v>
       </c>
@@ -35939,11 +35942,11 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="L102" s="8">
-        <f>ABS(K102-I102)</f>
+        <f t="shared" si="8"/>
         <v>4.6361086231775886E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>19</v>
       </c>
@@ -35966,11 +35969,11 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="L103" s="8">
-        <f>ABS(K103-I103)</f>
+        <f t="shared" si="8"/>
         <v>4.889411354928596E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>19</v>
       </c>
@@ -35993,11 +35996,11 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="L104" s="8">
-        <f>ABS(K104-I104)</f>
+        <f t="shared" si="8"/>
         <v>5.277062496890083E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>2391</v>
       </c>
@@ -36021,7 +36024,7 @@
       <c r="G105"/>
       <c r="H105" s="6"/>
     </row>
-    <row r="106" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>18</v>
       </c>
@@ -36041,11 +36044,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L106" s="8">
-        <f>ABS(K106-I106)</f>
+        <f t="shared" ref="L106:L153" si="9">ABS(K106-I106)</f>
         <v>0.37374142453591608</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>18</v>
       </c>
@@ -36065,11 +36068,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L107" s="8">
-        <f>ABS(K107-I107)</f>
+        <f t="shared" si="9"/>
         <v>0.2222886400322841</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>18</v>
       </c>
@@ -36079,7 +36082,7 @@
       <c r="H108" s="23">
         <v>10626</v>
       </c>
-      <c r="I108" s="7">
+      <c r="I108" s="25">
         <v>8.0402542372881358E-2</v>
       </c>
       <c r="J108" s="5">
@@ -36089,11 +36092,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L108" s="8">
-        <f>ABS(K108-I108)</f>
+        <f t="shared" si="9"/>
         <v>5.9569209039548029E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>18</v>
       </c>
@@ -36113,11 +36116,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L109" s="8">
-        <f>ABS(K109-I109)</f>
+        <f t="shared" si="9"/>
         <v>4.4239305891848289E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>18</v>
       </c>
@@ -36137,11 +36140,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L110" s="8">
-        <f>ABS(K110-I110)</f>
+        <f t="shared" si="9"/>
         <v>3.0619451170298649E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>18</v>
       </c>
@@ -36161,11 +36164,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L111" s="8">
-        <f>ABS(K111-I111)</f>
+        <f t="shared" si="9"/>
         <v>6.5577078288942686E-4</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>18</v>
       </c>
@@ -36185,11 +36188,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L112" s="8">
-        <f>ABS(K112-I112)</f>
+        <f t="shared" si="9"/>
         <v>3.7479822437449552E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>18</v>
       </c>
@@ -36209,11 +36212,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L113" s="8">
-        <f>ABS(K113-I113)</f>
+        <f t="shared" si="9"/>
         <v>3.8009483454398696E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>18</v>
       </c>
@@ -36233,11 +36236,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L114" s="8">
-        <f>ABS(K114-I114)</f>
+        <f t="shared" si="9"/>
         <v>5.0040355125100869E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -36257,11 +36260,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L115" s="8">
-        <f>ABS(K115-I115)</f>
+        <f t="shared" si="9"/>
         <v>5.5942292171105718E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>18</v>
       </c>
@@ -36281,11 +36284,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L116" s="8">
-        <f>ABS(K116-I116)</f>
+        <f t="shared" si="9"/>
         <v>6.0557909604519768E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>18</v>
       </c>
@@ -36305,11 +36308,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L117" s="8">
-        <f>ABS(K117-I117)</f>
+        <f t="shared" si="9"/>
         <v>6.9032485875706196E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -36329,11 +36332,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L118" s="8">
-        <f>ABS(K118-I118)</f>
+        <f t="shared" si="9"/>
         <v>7.0924132364810315E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>18</v>
       </c>
@@ -36353,11 +36356,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L119" s="8">
-        <f>ABS(K119-I119)</f>
+        <f t="shared" si="9"/>
         <v>8.1517352703793372E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>18</v>
       </c>
@@ -36377,11 +36380,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L120" s="8">
-        <f>ABS(K120-I120)</f>
+        <f t="shared" si="9"/>
         <v>1.1344834543987084E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>18</v>
       </c>
@@ -36401,11 +36404,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L121" s="8">
-        <f>ABS(K121-I121)</f>
+        <f t="shared" si="9"/>
         <v>1.341051251008878E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -36425,11 +36428,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L122" s="8">
-        <f>ABS(K122-I122)</f>
+        <f t="shared" si="9"/>
         <v>1.3569410815173526E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>18</v>
       </c>
@@ -36449,11 +36452,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L123" s="8">
-        <f>ABS(K123-I123)</f>
+        <f t="shared" si="9"/>
         <v>1.4083938660209846E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>18</v>
       </c>
@@ -36473,11 +36476,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L124" s="8">
-        <f>ABS(K124-I124)</f>
+        <f t="shared" si="9"/>
         <v>1.4295803066989507E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>18</v>
       </c>
@@ -36497,11 +36500,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L125" s="8">
-        <f>ABS(K125-I125)</f>
+        <f t="shared" si="9"/>
         <v>1.4560633575464083E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>18</v>
       </c>
@@ -36521,11 +36524,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L126" s="8">
-        <f>ABS(K126-I126)</f>
+        <f t="shared" si="9"/>
         <v>1.4893563357546408E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>18</v>
       </c>
@@ -36545,11 +36548,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L127" s="8">
-        <f>ABS(K127-I127)</f>
+        <f t="shared" si="9"/>
         <v>1.5968018563357545E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>18</v>
       </c>
@@ -36569,11 +36572,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L128" s="8">
-        <f>ABS(K128-I128)</f>
+        <f t="shared" si="9"/>
         <v>1.6739810330912024E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>18</v>
       </c>
@@ -36593,11 +36596,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L129" s="8">
-        <f>ABS(K129-I129)</f>
+        <f t="shared" si="9"/>
         <v>1.6860875706214688E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>18</v>
       </c>
@@ -36617,11 +36620,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L130" s="8">
-        <f>ABS(K130-I130)</f>
+        <f t="shared" si="9"/>
         <v>1.7224071832122677E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -36641,11 +36644,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L131" s="8">
-        <f>ABS(K131-I131)</f>
+        <f t="shared" si="9"/>
         <v>1.7451069410815173E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>18</v>
       </c>
@@ -36665,11 +36668,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L132" s="8">
-        <f>ABS(K132-I132)</f>
+        <f t="shared" si="9"/>
         <v>1.7473769168684421E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>18</v>
       </c>
@@ -36689,11 +36692,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L133" s="8">
-        <f>ABS(K133-I133)</f>
+        <f t="shared" si="9"/>
         <v>1.8253127522195316E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>18</v>
       </c>
@@ -36713,11 +36716,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L134" s="8">
-        <f>ABS(K134-I134)</f>
+        <f t="shared" si="9"/>
         <v>1.8434725585149313E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -36737,11 +36740,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L135" s="8">
-        <f>ABS(K135-I135)</f>
+        <f t="shared" si="9"/>
         <v>1.8540657788539142E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>18</v>
       </c>
@@ -36761,11 +36764,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L136" s="8">
-        <f>ABS(K136-I136)</f>
+        <f t="shared" si="9"/>
         <v>1.8843321226795801E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>18</v>
       </c>
@@ -36785,11 +36788,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L137" s="8">
-        <f>ABS(K137-I137)</f>
+        <f t="shared" si="9"/>
         <v>1.9471347861178368E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>18</v>
       </c>
@@ -36809,11 +36812,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L138" s="8">
-        <f>ABS(K138-I138)</f>
+        <f t="shared" si="9"/>
         <v>1.9683212267958029E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>18</v>
       </c>
@@ -36833,11 +36836,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L139" s="8">
-        <f>ABS(K139-I139)</f>
+        <f t="shared" si="9"/>
         <v>1.9683212267958029E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>18</v>
       </c>
@@ -36857,11 +36860,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L140" s="8">
-        <f>ABS(K140-I140)</f>
+        <f t="shared" si="9"/>
         <v>1.9789144471347862E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>18</v>
       </c>
@@ -36881,11 +36884,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L141" s="8">
-        <f>ABS(K141-I141)</f>
+        <f t="shared" si="9"/>
         <v>1.9819410815173525E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>18</v>
       </c>
@@ -36905,11 +36908,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L142" s="8">
-        <f>ABS(K142-I142)</f>
+        <f t="shared" si="9"/>
         <v>2.0205306698950765E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>18</v>
       </c>
@@ -36929,11 +36932,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L143" s="8">
-        <f>ABS(K143-I143)</f>
+        <f t="shared" si="9"/>
         <v>2.0432304277643261E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -36953,11 +36956,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L144" s="8">
-        <f>ABS(K144-I144)</f>
+        <f t="shared" si="9"/>
         <v>2.0492836965294591E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>18</v>
       </c>
@@ -36977,11 +36980,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L145" s="8">
-        <f>ABS(K145-I145)</f>
+        <f t="shared" si="9"/>
         <v>2.0492836965294591E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>18</v>
       </c>
@@ -37001,11 +37004,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L146" s="8">
-        <f>ABS(K146-I146)</f>
+        <f t="shared" si="9"/>
         <v>2.0523103309120258E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>18</v>
       </c>
@@ -37025,11 +37028,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L147" s="8">
-        <f>ABS(K147-I147)</f>
+        <f t="shared" si="9"/>
         <v>2.0530669895076674E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>18</v>
       </c>
@@ -37049,11 +37052,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L148" s="8">
-        <f>ABS(K148-I148)</f>
+        <f t="shared" si="9"/>
         <v>2.0568502824858757E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>18</v>
       </c>
@@ -37073,11 +37076,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L149" s="8">
-        <f>ABS(K149-I149)</f>
+        <f t="shared" si="9"/>
         <v>2.066686844229217E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>18</v>
       </c>
@@ -37097,11 +37100,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L150" s="8">
-        <f>ABS(K150-I150)</f>
+        <f t="shared" si="9"/>
         <v>2.0719834543987084E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>18</v>
       </c>
@@ -37121,11 +37124,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L151" s="8">
-        <f>ABS(K151-I151)</f>
+        <f t="shared" si="9"/>
         <v>2.0742534301856335E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>18</v>
       </c>
@@ -37145,11 +37148,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L152" s="8">
-        <f>ABS(K152-I152)</f>
+        <f t="shared" si="9"/>
         <v>2.0795500403551249E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>18</v>
       </c>
@@ -37169,11 +37172,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="L153" s="8">
-        <f>ABS(K153-I153)</f>
+        <f t="shared" si="9"/>
         <v>2.0825766747376916E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>2392</v>
       </c>
@@ -37197,7 +37200,7 @@
       <c r="G154"/>
       <c r="H154" s="6"/>
     </row>
-    <row r="155" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>30</v>
       </c>
@@ -37217,11 +37220,11 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="L155" s="8">
-        <f>ABS(K155-I155)</f>
+        <f t="shared" ref="L155:L161" si="10">ABS(K155-I155)</f>
         <v>0.52406181697418108</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>30</v>
       </c>
@@ -37231,7 +37234,7 @@
       <c r="H156" s="23">
         <v>8376</v>
       </c>
-      <c r="I156" s="7">
+      <c r="I156" s="25">
         <v>0.11320754716981132</v>
       </c>
       <c r="J156" s="5">
@@ -37241,11 +37244,11 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="L156" s="8">
-        <f>ABS(K156-I156)</f>
+        <f t="shared" si="10"/>
         <v>2.9649595687331526E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>30</v>
       </c>
@@ -37265,11 +37268,11 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="L157" s="8">
-        <f>ABS(K157-I157)</f>
+        <f t="shared" si="10"/>
         <v>3.4528765282400994E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>30</v>
       </c>
@@ -37289,11 +37292,11 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="L158" s="8">
-        <f>ABS(K158-I158)</f>
+        <f t="shared" si="10"/>
         <v>7.9698252226229727E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>30</v>
       </c>
@@ -37313,11 +37316,11 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="L159" s="8">
-        <f>ABS(K159-I159)</f>
+        <f t="shared" si="10"/>
         <v>0.10744599510345307</v>
       </c>
     </row>
-    <row r="160" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>30</v>
       </c>
@@ -37337,11 +37340,11 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="L160" s="8">
-        <f>ABS(K160-I160)</f>
+        <f t="shared" si="10"/>
         <v>0.1343152171394589</v>
       </c>
     </row>
-    <row r="161" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>30</v>
       </c>
@@ -37361,11 +37364,11 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="L161" s="8">
-        <f>ABS(K161-I161)</f>
+        <f t="shared" si="10"/>
         <v>0.13842399153530688</v>
       </c>
     </row>
-    <row r="162" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>2393</v>
       </c>
@@ -37389,7 +37392,7 @@
       <c r="G162"/>
       <c r="H162" s="6"/>
     </row>
-    <row r="163" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>50</v>
       </c>
@@ -37402,7 +37405,7 @@
       <c r="H163" s="23">
         <v>32840</v>
       </c>
-      <c r="I163" s="7">
+      <c r="I163" s="25">
         <v>1</v>
       </c>
       <c r="J163" s="5">
@@ -37412,11 +37415,11 @@
         <v>1</v>
       </c>
       <c r="L163" s="8">
-        <f t="shared" ref="L163:L194" si="4">ABS(K163-I163)</f>
+        <f t="shared" ref="L163:L194" si="11">ABS(K163-I163)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>2394</v>
       </c>
@@ -37440,7 +37443,7 @@
       <c r="G164"/>
       <c r="H164" s="6"/>
     </row>
-    <row r="165" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>43</v>
       </c>
@@ -37450,7 +37453,7 @@
       <c r="H165" s="23">
         <v>556</v>
       </c>
-      <c r="I165" s="7">
+      <c r="I165" s="25">
         <v>1</v>
       </c>
       <c r="J165" s="5">
@@ -37460,11 +37463,11 @@
         <v>1</v>
       </c>
       <c r="L165" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>2395</v>
       </c>
@@ -37488,7 +37491,7 @@
       <c r="G166"/>
       <c r="H166" s="6"/>
     </row>
-    <row r="167" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>7</v>
       </c>
@@ -37500,7 +37503,7 @@
       <c r="H167" s="23">
         <v>855</v>
       </c>
-      <c r="I167" s="7">
+      <c r="I167" s="25">
         <v>1</v>
       </c>
       <c r="J167" s="5">
@@ -37510,11 +37513,11 @@
         <v>1</v>
       </c>
       <c r="L167" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>1400</v>
       </c>
@@ -37538,7 +37541,7 @@
       <c r="G168"/>
       <c r="H168" s="6"/>
     </row>
-    <row r="169" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -37551,7 +37554,7 @@
       <c r="H169" s="23">
         <v>85334</v>
       </c>
-      <c r="I169" s="7">
+      <c r="I169" s="25">
         <v>1</v>
       </c>
       <c r="J169" s="5">
@@ -37561,11 +37564,11 @@
         <v>1</v>
       </c>
       <c r="L169" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>2396</v>
       </c>
@@ -37589,7 +37592,7 @@
       <c r="G170"/>
       <c r="H170" s="6"/>
     </row>
-    <row r="171" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>34</v>
       </c>
@@ -37609,11 +37612,11 @@
         <v>0.125</v>
       </c>
       <c r="L171" s="8">
-        <f>ABS(K171-I171)</f>
+        <f t="shared" ref="L171:L178" si="12">ABS(K171-I171)</f>
         <v>0.43801609808991571</v>
       </c>
     </row>
-    <row r="172" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>34</v>
       </c>
@@ -37633,11 +37636,11 @@
         <v>0.125</v>
       </c>
       <c r="L172" s="8">
-        <f>ABS(K172-I172)</f>
+        <f t="shared" si="12"/>
         <v>5.2162398865626819E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>34</v>
       </c>
@@ -37657,11 +37660,11 @@
         <v>0.125</v>
       </c>
       <c r="L173" s="8">
-        <f>ABS(K173-I173)</f>
+        <f t="shared" si="12"/>
         <v>4.1256568521144385E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>34</v>
       </c>
@@ -37681,11 +37684,11 @@
         <v>0.125</v>
       </c>
       <c r="L174" s="8">
-        <f>ABS(K174-I174)</f>
+        <f t="shared" si="12"/>
         <v>4.3508632913504042E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>34</v>
       </c>
@@ -37705,11 +37708,11 @@
         <v>0.125</v>
       </c>
       <c r="L175" s="8">
-        <f>ABS(K175-I175)</f>
+        <f t="shared" si="12"/>
         <v>7.4120026691133545E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>34</v>
       </c>
@@ -37729,11 +37732,11 @@
         <v>0.125</v>
       </c>
       <c r="L176" s="8">
-        <f>ABS(K176-I176)</f>
+        <f t="shared" si="12"/>
         <v>0.10289640503795146</v>
       </c>
     </row>
-    <row r="177" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>34</v>
       </c>
@@ -37743,7 +37746,7 @@
       <c r="H177" s="23">
         <v>216</v>
       </c>
-      <c r="I177" s="7">
+      <c r="I177" s="25">
         <v>1.8016515138877306E-2</v>
       </c>
       <c r="J177" s="5">
@@ -37753,11 +37756,11 @@
         <v>0.125</v>
       </c>
       <c r="L177" s="8">
-        <f>ABS(K177-I177)</f>
+        <f t="shared" si="12"/>
         <v>0.10698348486112269</v>
       </c>
     </row>
-    <row r="178" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>34</v>
       </c>
@@ -37777,11 +37780,11 @@
         <v>0.125</v>
       </c>
       <c r="L178" s="8">
-        <f>ABS(K178-I178)</f>
+        <f t="shared" si="12"/>
         <v>0.12141337893068646</v>
       </c>
     </row>
-    <row r="179" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>2397</v>
       </c>
@@ -37805,7 +37808,7 @@
       <c r="G179"/>
       <c r="H179" s="6"/>
     </row>
-    <row r="180" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>28</v>
       </c>
@@ -37818,7 +37821,7 @@
       <c r="H180" s="23">
         <v>3794</v>
       </c>
-      <c r="I180" s="7">
+      <c r="I180" s="25">
         <v>0.32006073899105786</v>
       </c>
       <c r="J180" s="5">
@@ -37828,11 +37831,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="L180" s="8">
-        <f>ABS(K180-I180)</f>
+        <f t="shared" ref="L180:L188" si="13">ABS(K180-I180)</f>
         <v>0.20894962787994675</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>28</v>
       </c>
@@ -37855,11 +37858,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="L181" s="8">
-        <f>ABS(K181-I181)</f>
+        <f t="shared" si="13"/>
         <v>0.13057945747333297</v>
       </c>
     </row>
-    <row r="182" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>28</v>
       </c>
@@ -37882,11 +37885,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="L182" s="8">
-        <f>ABS(K182-I182)</f>
+        <f t="shared" si="13"/>
         <v>0.1040905085953171</v>
       </c>
     </row>
-    <row r="183" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>28</v>
       </c>
@@ -37909,11 +37912,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="L183" s="8">
-        <f>ABS(K183-I183)</f>
+        <f t="shared" si="13"/>
         <v>3.7886883002455796E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>28</v>
       </c>
@@ -37936,11 +37939,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="L184" s="8">
-        <f>ABS(K184-I184)</f>
+        <f t="shared" si="13"/>
         <v>4.3285904429822095E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>28</v>
       </c>
@@ -37963,11 +37966,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="L185" s="8">
-        <f>ABS(K185-I185)</f>
+        <f t="shared" si="13"/>
         <v>8.3103687456648478E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>28</v>
       </c>
@@ -37990,11 +37993,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="L186" s="8">
-        <f>ABS(K186-I186)</f>
+        <f t="shared" si="13"/>
         <v>8.4116003974279652E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>28</v>
       </c>
@@ -38017,11 +38020,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="L187" s="8">
-        <f>ABS(K187-I187)</f>
+        <f t="shared" si="13"/>
         <v>8.6984234107568004E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>28</v>
       </c>
@@ -38044,11 +38047,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="L188" s="8">
-        <f>ABS(K188-I188)</f>
+        <f t="shared" si="13"/>
         <v>0.10824288097782277</v>
       </c>
     </row>
-    <row r="189" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>2398</v>
       </c>
@@ -38085,7 +38088,7 @@
       <c r="H190" s="23">
         <v>158</v>
       </c>
-      <c r="I190" s="7">
+      <c r="I190" s="25">
         <v>1</v>
       </c>
       <c r="J190" s="5">
@@ -38095,7 +38098,7 @@
         <v>1</v>
       </c>
       <c r="L190" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -38136,7 +38139,7 @@
       <c r="H192" s="23">
         <v>218</v>
       </c>
-      <c r="I192" s="7">
+      <c r="I192" s="25">
         <v>1</v>
       </c>
       <c r="J192" s="5">
@@ -38146,7 +38149,7 @@
         <v>1</v>
       </c>
       <c r="L192" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -38187,7 +38190,7 @@
       <c r="H194" s="23">
         <v>147</v>
       </c>
-      <c r="I194" s="7">
+      <c r="I194" s="25">
         <v>1</v>
       </c>
       <c r="J194" s="5">
@@ -38197,7 +38200,7 @@
         <v>1</v>
       </c>
       <c r="L194" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -38225,7 +38228,7 @@
       <c r="G195"/>
       <c r="H195" s="6"/>
     </row>
-    <row r="196" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>9</v>
       </c>
@@ -38237,7 +38240,7 @@
       <c r="H196" s="23">
         <v>1641</v>
       </c>
-      <c r="I196" s="7">
+      <c r="I196" s="25">
         <v>1</v>
       </c>
       <c r="J196" s="5">
@@ -38247,11 +38250,11 @@
         <v>1</v>
       </c>
       <c r="L196" s="8">
-        <f t="shared" ref="L196:L199" si="5">ABS(K196-I196)</f>
+        <f t="shared" ref="L196:L199" si="14">ABS(K196-I196)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>1436</v>
       </c>
@@ -38275,7 +38278,7 @@
       <c r="G197"/>
       <c r="H197" s="6"/>
     </row>
-    <row r="198" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>38</v>
       </c>
@@ -38288,7 +38291,7 @@
       <c r="H198" s="23">
         <v>14185</v>
       </c>
-      <c r="I198" s="7">
+      <c r="I198" s="25">
         <v>0.77918154353199676</v>
       </c>
       <c r="J198" s="5">
@@ -38302,7 +38305,7 @@
         <v>0.27918154353199676</v>
       </c>
     </row>
-    <row r="199" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>38</v>
       </c>
@@ -38325,11 +38328,11 @@
         <v>0.5</v>
       </c>
       <c r="L199" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0.2791815435319967</v>
       </c>
     </row>
-    <row r="200" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>2402</v>
       </c>
@@ -38353,7 +38356,7 @@
       <c r="G200"/>
       <c r="H200" s="6"/>
     </row>
-    <row r="201" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>21</v>
       </c>
@@ -38373,11 +38376,11 @@
         <v>0.6</v>
       </c>
       <c r="L201" s="8">
-        <f t="shared" ref="L201:L219" si="6">ABS(K201-I201)</f>
+        <f t="shared" ref="L201:L219" si="15">ABS(K201-I201)</f>
         <v>0.56144436007761744</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>21</v>
       </c>
@@ -38397,11 +38400,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L202" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.48892263561967436</v>
       </c>
     </row>
-    <row r="203" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>21</v>
       </c>
@@ -38421,11 +38424,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L203" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.18376782249219606</v>
       </c>
     </row>
-    <row r="204" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>21</v>
       </c>
@@ -38445,11 +38448,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L204" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>9.5671981776765377E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>21</v>
       </c>
@@ -38469,11 +38472,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L205" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>5.7909390027841054E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>21</v>
       </c>
@@ -38493,11 +38496,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L206" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2.1935375010545856E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>21</v>
       </c>
@@ -38517,11 +38520,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L207" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2.1884754914367671E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>21</v>
       </c>
@@ -38541,11 +38544,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L208" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2.1209820298658567E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>21</v>
       </c>
@@ -38565,11 +38568,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L209" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2.1024213279338566E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>21</v>
       </c>
@@ -38589,11 +38592,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L210" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2.0956719817767654E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>21</v>
       </c>
@@ -38613,11 +38616,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L211" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2.0804859529233107E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>21</v>
       </c>
@@ -38637,11 +38640,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L212" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2.0602379144520375E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>21</v>
       </c>
@@ -38661,11 +38664,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L213" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2.0551759048342194E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>21</v>
       </c>
@@ -38685,11 +38688,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L214" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2.0501138952164009E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>21</v>
       </c>
@@ -38709,11 +38712,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L215" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>1.9522483759385811E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>21</v>
       </c>
@@ -38733,11 +38736,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L216" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>1.8712562220534888E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>21</v>
       </c>
@@ -38757,11 +38760,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L217" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>1.8577575297393067E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>21</v>
       </c>
@@ -38781,11 +38784,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L218" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>1.6620264911836668E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>21</v>
       </c>
@@ -38795,7 +38798,7 @@
       <c r="H219" s="23">
         <v>1203</v>
       </c>
-      <c r="I219" s="7">
+      <c r="I219" s="25">
         <v>2.0298658567451278E-2</v>
       </c>
       <c r="J219" s="5">
@@ -38805,11 +38808,11 @@
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="L219" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>1.9235636547709455E-3</v>
       </c>
     </row>
-    <row r="220" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>2403</v>
       </c>
@@ -38833,7 +38836,7 @@
       <c r="G220"/>
       <c r="H220" s="6"/>
     </row>
-    <row r="221" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>20</v>
       </c>
@@ -38843,7 +38846,7 @@
       <c r="H221" s="23">
         <v>157430</v>
       </c>
-      <c r="I221" s="7">
+      <c r="I221" s="25">
         <v>0.99521452458166604</v>
       </c>
       <c r="J221" s="5">
@@ -38853,11 +38856,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L221" s="8">
-        <f t="shared" ref="L221:L237" si="7">ABS(K221-I221)</f>
+        <f t="shared" ref="L221:L237" si="16">ABS(K221-I221)</f>
         <v>0.93639099516990132</v>
       </c>
     </row>
-    <row r="222" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>20</v>
       </c>
@@ -38877,11 +38880,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L222" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.880456451578716E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>20</v>
       </c>
@@ -38901,11 +38904,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L223" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8798242883794642E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>20</v>
       </c>
@@ -38925,11 +38928,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L224" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8798242883794642E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>20</v>
       </c>
@@ -38949,11 +38952,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L225" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8798242883794642E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>20</v>
       </c>
@@ -38973,11 +38976,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L226" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8791921251802132E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>20</v>
       </c>
@@ -38997,11 +39000,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L227" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8772956355824586E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>20</v>
       </c>
@@ -39021,11 +39024,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L228" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8772956355824586E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>20</v>
       </c>
@@ -39045,11 +39048,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L229" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8753991459847041E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>20</v>
       </c>
@@ -39069,11 +39072,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L230" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8728704931876978E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>20</v>
       </c>
@@ -39093,11 +39096,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L231" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8583307396049125E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>20</v>
       </c>
@@ -39117,11 +39120,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L232" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8539055972101524E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>20</v>
       </c>
@@ -39141,11 +39144,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L233" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8488482916161398E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>20</v>
       </c>
@@ -39165,11 +39168,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L234" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8450553124206307E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>20</v>
       </c>
@@ -39189,11 +39192,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L235" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.8343085380333552E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>20</v>
       </c>
@@ -39213,11 +39216,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L236" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.7514951589314064E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>20</v>
       </c>
@@ -39237,11 +39240,11 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="L237" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>5.7451735269388911E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>2404</v>
       </c>
@@ -39265,7 +39268,7 @@
       <c r="G238"/>
       <c r="H238" s="6"/>
     </row>
-    <row r="239" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>27</v>
       </c>
@@ -39288,11 +39291,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L239" s="8">
-        <f t="shared" ref="L239:L251" si="8">ABS(K239-I239)</f>
+        <f t="shared" ref="L239:L251" si="17">ABS(K239-I239)</f>
         <v>0.20167883325778063</v>
       </c>
     </row>
-    <row r="240" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>27</v>
       </c>
@@ -39315,11 +39318,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L240" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0.15941100151626467</v>
       </c>
     </row>
-    <row r="241" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>27</v>
       </c>
@@ -39342,11 +39345,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L241" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0.11822696033222349</v>
       </c>
     </row>
-    <row r="242" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>27</v>
       </c>
@@ -39369,11 +39372,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L242" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>7.6042497095128683E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>27</v>
       </c>
@@ -39396,11 +39399,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L243" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>7.5263522631943691E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>27</v>
       </c>
@@ -39423,11 +39426,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L244" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>7.5128048812259346E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>27</v>
       </c>
@@ -39450,11 +39453,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L245" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>7.1910545594756126E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>27</v>
       </c>
@@ -39467,7 +39470,7 @@
       <c r="H246" s="23">
         <v>257</v>
       </c>
-      <c r="I246" s="7">
+      <c r="I246" s="25">
         <v>8.7041929147192304E-3</v>
       </c>
       <c r="J246" s="5">
@@ -39477,11 +39480,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L246" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>6.8218884008357697E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>27</v>
       </c>
@@ -39504,11 +39507,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L247" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>6.3985327143221887E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>27</v>
       </c>
@@ -39531,11 +39534,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L248" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>4.5899572215361693E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>27</v>
       </c>
@@ -39558,11 +39561,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L249" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1.612920033972666E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>27</v>
       </c>
@@ -39585,11 +39588,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L250" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>7.3416389205862853E-3</v>
       </c>
     </row>
-    <row r="251" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>27</v>
       </c>
@@ -39612,11 +39615,11 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="L251" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>5.9191638139006464E-3</v>
       </c>
     </row>
-    <row r="252" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>2405</v>
       </c>
@@ -39640,7 +39643,7 @@
       <c r="G252"/>
       <c r="H252" s="6"/>
     </row>
-    <row r="253" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>33</v>
       </c>
@@ -39650,7 +39653,7 @@
       <c r="H253" s="23">
         <v>276</v>
       </c>
-      <c r="I253" s="7">
+      <c r="I253" s="25">
         <v>0.57983193277310929</v>
       </c>
       <c r="J253" s="5">
@@ -39664,7 +39667,7 @@
         <v>0.37983193277310928</v>
       </c>
     </row>
-    <row r="254" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>33</v>
       </c>
@@ -39688,7 +39691,7 @@
         <v>0.18739495798319328</v>
       </c>
     </row>
-    <row r="255" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>33</v>
       </c>
@@ -39712,7 +39715,7 @@
         <v>0.10756302521008404</v>
       </c>
     </row>
-    <row r="256" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>33</v>
       </c>
@@ -39736,7 +39739,7 @@
         <v>6.5546218487394975E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>33</v>
       </c>
@@ -39760,7 +39763,7 @@
         <v>1.9327731092436989E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>2406</v>
       </c>
@@ -39784,7 +39787,7 @@
       <c r="G258"/>
       <c r="H258" s="6"/>
     </row>
-    <row r="259" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>41</v>
       </c>
@@ -39797,7 +39800,7 @@
       <c r="H259" s="23">
         <v>282</v>
       </c>
-      <c r="I259" s="7">
+      <c r="I259" s="25">
         <v>1</v>
       </c>
       <c r="J259" s="5">
@@ -39807,11 +39810,11 @@
         <v>1</v>
       </c>
       <c r="L259" s="8">
-        <f t="shared" ref="L259:L302" si="9">ABS(K259-I259)</f>
+        <f t="shared" ref="L259:L302" si="18">ABS(K259-I259)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>2407</v>
       </c>
@@ -39835,7 +39838,7 @@
       <c r="G260"/>
       <c r="H260" s="6"/>
     </row>
-    <row r="261" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="s">
         <v>14</v>
       </c>
@@ -39847,7 +39850,7 @@
       <c r="H261" s="23">
         <v>20800</v>
       </c>
-      <c r="I261" s="7">
+      <c r="I261" s="25">
         <v>1</v>
       </c>
       <c r="J261" s="5">
@@ -39857,11 +39860,11 @@
         <v>1</v>
       </c>
       <c r="L261" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>1637</v>
       </c>
@@ -39885,7 +39888,7 @@
       <c r="G262"/>
       <c r="H262" s="6"/>
     </row>
-    <row r="263" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>17</v>
       </c>
@@ -39895,7 +39898,7 @@
       <c r="H263" s="23">
         <v>31590</v>
       </c>
-      <c r="I263" s="7">
+      <c r="I263" s="25">
         <v>0.73665555115080572</v>
       </c>
       <c r="J263" s="5">
@@ -39905,11 +39908,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L263" s="8">
-        <f t="shared" ref="L263:L283" si="10">ABS(K263-I263)</f>
+        <f t="shared" ref="L263:L283" si="19">ABS(K263-I263)</f>
         <v>0.68903650353175805</v>
       </c>
     </row>
-    <row r="264" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>17</v>
       </c>
@@ -39929,11 +39932,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L264" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>8.7959153532924023E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>17</v>
       </c>
@@ -39953,11 +39956,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L265" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.7269258658387214E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>17</v>
       </c>
@@ -39977,11 +39980,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L266" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.7245939394343191E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>17</v>
       </c>
@@ -40001,11 +40004,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L267" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.7245939394343191E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>17</v>
       </c>
@@ -40025,11 +40028,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L268" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.7082704546034998E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>17</v>
       </c>
@@ -40049,11 +40052,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L269" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.6966108225814866E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>17</v>
       </c>
@@ -40073,11 +40076,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L270" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.6289849568538093E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>17</v>
       </c>
@@ -40097,11 +40100,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L271" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.6056656928097822E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>17</v>
       </c>
@@ -40121,11 +40124,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L272" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.594006060787769E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>17</v>
       </c>
@@ -40145,11 +40148,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L273" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.5473675326997157E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>17</v>
       </c>
@@ -40169,11 +40172,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L274" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.4610862557368167E-2</v>
       </c>
     </row>
-    <row r="275" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>17</v>
       </c>
@@ -40193,11 +40196,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L275" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.4587543293324136E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>17</v>
       </c>
@@ -40217,11 +40220,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L276" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.4377669916927896E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>17</v>
       </c>
@@ -40241,11 +40244,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L277" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.4027880956267494E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>17</v>
       </c>
@@ -40265,11 +40268,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L278" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>4.311842965855045E-2</v>
       </c>
     </row>
-    <row r="279" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>17</v>
       </c>
@@ -40289,11 +40292,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L279" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>3.901423918680174E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>17</v>
       </c>
@@ -40313,11 +40316,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L280" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>3.8221384209304828E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>17</v>
       </c>
@@ -40337,11 +40340,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L281" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>3.5446391788065641E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>17</v>
       </c>
@@ -40361,11 +40364,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L282" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>1.3946030339472962E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>17</v>
       </c>
@@ -40385,11 +40388,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L283" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>1.0075032508164515E-2</v>
       </c>
     </row>
-    <row r="284" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>2408</v>
       </c>
@@ -40413,7 +40416,7 @@
       <c r="G284"/>
       <c r="H284" s="6"/>
     </row>
-    <row r="285" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>44</v>
       </c>
@@ -40423,7 +40426,7 @@
       <c r="H285" s="23">
         <v>47528</v>
       </c>
-      <c r="I285" s="7">
+      <c r="I285" s="25">
         <v>1</v>
       </c>
       <c r="J285" s="5">
@@ -40433,11 +40436,11 @@
         <v>1</v>
       </c>
       <c r="L285" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>2409</v>
       </c>
@@ -40461,7 +40464,7 @@
       <c r="G286"/>
       <c r="H286" s="6"/>
     </row>
-    <row r="287" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>23</v>
       </c>
@@ -40481,11 +40484,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L287" s="8">
-        <f t="shared" ref="L287:L298" si="11">ABS(K287-I287)</f>
+        <f t="shared" ref="L287:L298" si="20">ABS(K287-I287)</f>
         <v>0.15660935942220902</v>
       </c>
     </row>
-    <row r="288" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>23</v>
       </c>
@@ -40505,11 +40508,11 @@
         <v>0.42857142857142855</v>
       </c>
       <c r="L288" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>0.13954656499006823</v>
       </c>
     </row>
-    <row r="289" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>23</v>
       </c>
@@ -40529,11 +40532,11 @@
         <v>9.5238095238095233E-2</v>
       </c>
       <c r="L289" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>7.8441669140086906E-2</v>
       </c>
     </row>
-    <row r="290" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>23</v>
       </c>
@@ -40553,11 +40556,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L290" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>4.0632586740945373E-2</v>
       </c>
     </row>
-    <row r="291" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>23</v>
       </c>
@@ -40577,11 +40580,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L291" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>3.9483397642259721E-2</v>
       </c>
     </row>
-    <row r="292" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>23</v>
       </c>
@@ -40591,7 +40594,7 @@
       <c r="H292" s="23">
         <v>487</v>
       </c>
-      <c r="I292" s="7">
+      <c r="I292" s="25">
         <v>1.1118975319071212E-2</v>
       </c>
       <c r="J292" s="5">
@@ -40601,11 +40604,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L292" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>3.6500072299976406E-2</v>
       </c>
     </row>
-    <row r="293" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>23</v>
       </c>
@@ -40625,11 +40628,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L293" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>3.5084514867158301E-2</v>
       </c>
     </row>
-    <row r="294" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>23</v>
       </c>
@@ -40649,11 +40652,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L294" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>2.5015791836952135E-2</v>
       </c>
     </row>
-    <row r="295" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>23</v>
       </c>
@@ -40673,11 +40676,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L295" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>2.4460223597190203E-2</v>
       </c>
     </row>
-    <row r="296" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>23</v>
       </c>
@@ -40697,11 +40700,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L296" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>2.2755466258742585E-2</v>
       </c>
     </row>
-    <row r="297" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>23</v>
       </c>
@@ -40721,11 +40724,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L297" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>1.224533284625981E-2</v>
       </c>
     </row>
-    <row r="298" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>23</v>
       </c>
@@ -40745,11 +40748,11 @@
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="L298" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>1.1704985654162572E-2</v>
       </c>
     </row>
-    <row r="299" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>2410</v>
       </c>
@@ -40773,7 +40776,7 @@
       <c r="G299"/>
       <c r="H299" s="6"/>
     </row>
-    <row r="300" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A300" s="3" t="s">
         <v>15</v>
       </c>
@@ -40785,7 +40788,7 @@
       <c r="H300" s="23">
         <v>42125</v>
       </c>
-      <c r="I300" s="7">
+      <c r="I300" s="25">
         <v>1</v>
       </c>
       <c r="J300" s="5">
@@ -40795,11 +40798,11 @@
         <v>1</v>
       </c>
       <c r="L300" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>1705</v>
       </c>
@@ -40823,7 +40826,7 @@
       <c r="G301"/>
       <c r="H301" s="6"/>
     </row>
-    <row r="302" spans="1:12" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>47</v>
       </c>
@@ -40836,7 +40839,7 @@
       <c r="H302" s="23">
         <v>13165</v>
       </c>
-      <c r="I302" s="7">
+      <c r="I302" s="25">
         <v>1</v>
       </c>
       <c r="J302" s="5">
@@ -40846,11 +40849,11 @@
         <v>1</v>
       </c>
       <c r="L302" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:12" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>2411</v>
       </c>

</xml_diff>